<commit_message>
Add analysis of us delay function in head array
</commit_message>
<xml_diff>
--- a/HeadArray/HA_HHP_HeadArrayTimingAnalysis.xlsx
+++ b/HeadArray/HA_HHP_HeadArrayTimingAnalysis.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpars\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Invacare\ASL110\ASL110_Documentation\HeadArray\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC926DC5-7ADD-41D5-8312-17E053873E22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2965D2E-72B4-416E-ADC9-735EF1FD3512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1CC3B75C-6B58-4B8C-B05F-04D899897821}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{1CC3B75C-6B58-4B8C-B05F-04D899897821}"/>
   </bookViews>
   <sheets>
     <sheet name="SingleFunc" sheetId="1" r:id="rId1"/>
     <sheet name="SepFuncInline" sheetId="2" r:id="rId2"/>
     <sheet name="DelayCalcs" sheetId="3" r:id="rId3"/>
+    <sheet name="usDelayMeasuredData" sheetId="4" r:id="rId4"/>
+    <sheet name="usDelayVals" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
   <si>
     <t>Optimization 2 (w/ or w/o focus on Debug)</t>
   </si>
@@ -91,6 +93,15 @@
   <si>
     <t>Delay (us)</t>
   </si>
+  <si>
+    <t>Time to turn drive test GPIO low</t>
+  </si>
+  <si>
+    <t>Optimization 0 (Measured)</t>
+  </si>
+  <si>
+    <t>Optimization 2 (Measured)</t>
+  </si>
 </sst>
 </file>
 
@@ -113,12 +124,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="21">
@@ -413,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -473,22 +490,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -500,12 +508,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,7 +841,7 @@
   <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C9"/>
+      <selection activeCell="A2" sqref="A2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1037,7 @@
   <dimension ref="B1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B24" sqref="B24:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,44 +1059,44 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
       <c r="M2" s="30"/>
       <c r="N2" s="31"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="15"/>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="27" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="26" t="s">
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="26" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="24"/>
-      <c r="N3" s="25"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="23"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -1417,44 +1435,44 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
       <c r="M12" s="30"/>
       <c r="N12" s="31"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="26" t="s">
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26" t="s">
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="23"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="26" t="s">
+      <c r="J13" s="22"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
@@ -1826,11 +1844,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="B2:N2"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B12:N12"/>
@@ -1838,6 +1851,11 @@
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="L13:N13"/>
     <mergeCell ref="B13:E13"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="B2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1847,7 +1865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31877AB-3481-44BD-9C84-C79917CD6E2E}">
   <dimension ref="C1:E257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -5193,4 +5211,3148 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9918BCC6-78DB-4BFB-93F8-A53989EA45CB}">
+  <dimension ref="A3:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>38</v>
+      </c>
+      <c r="F6">
+        <f>E6-E5</f>
+        <v>3.2000000000000028</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>29.2</v>
+      </c>
+      <c r="I6">
+        <f>H6-H5</f>
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGE(I6:I9)</f>
+        <v>2.8000000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>41.2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F10" si="0">E7-E6</f>
+        <v>3.2000000000000028</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>32</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I10" si="1">H7-H6</f>
+        <v>2.8000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>44.4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>3.1999999999999957</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>34.9</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>2.8999999999999986</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>47.6</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>3.2000000000000028</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>37.6</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>2.7000000000000028</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>256</v>
+      </c>
+      <c r="E10">
+        <v>2098.1</v>
+      </c>
+      <c r="G10">
+        <v>256</v>
+      </c>
+      <c r="H10">
+        <v>2001.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>257</v>
+      </c>
+      <c r="E11">
+        <v>2107.4</v>
+      </c>
+      <c r="F11">
+        <f>E11-E10</f>
+        <v>9.3000000000001819</v>
+      </c>
+      <c r="G11">
+        <v>257</v>
+      </c>
+      <c r="H11">
+        <v>2010.6</v>
+      </c>
+      <c r="I11">
+        <f>H11-H10</f>
+        <v>8.8999999999998636</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE(I11:I14)</f>
+        <v>8.8000000000000114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="D12">
+        <v>258</v>
+      </c>
+      <c r="E12">
+        <v>2116.5</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F14" si="2">E12-E11</f>
+        <v>9.0999999999999091</v>
+      </c>
+      <c r="G12">
+        <v>258</v>
+      </c>
+      <c r="H12">
+        <v>2019.3</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I14" si="3">H12-H11</f>
+        <v>8.7000000000000455</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="D13">
+        <v>259</v>
+      </c>
+      <c r="E13">
+        <v>2125.8000000000002</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>9.3000000000001819</v>
+      </c>
+      <c r="G13">
+        <v>259</v>
+      </c>
+      <c r="H13">
+        <v>2028.2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>8.9000000000000909</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>260</v>
+      </c>
+      <c r="E14">
+        <v>2134.9</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>9.0999999999999091</v>
+      </c>
+      <c r="G14">
+        <v>260</v>
+      </c>
+      <c r="H14">
+        <v>2036.9</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>8.7000000000000455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14.8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="D3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0DA5376-D526-4E3D-8F29-82390A896260}">
+  <dimension ref="B1:D257"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D163" activeCellId="1" sqref="C140 D163"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="D2">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>41.2</v>
+      </c>
+      <c r="D4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>44.4</v>
+      </c>
+      <c r="D5" s="32">
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>47.6</v>
+      </c>
+      <c r="D6">
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="32">
+        <v>50.8</v>
+      </c>
+      <c r="D7">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>54</v>
+      </c>
+      <c r="D8">
+        <v>43.2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>57.2</v>
+      </c>
+      <c r="D9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>60.4</v>
+      </c>
+      <c r="D10">
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>63.6</v>
+      </c>
+      <c r="D11" s="32">
+        <v>51.6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>66.8</v>
+      </c>
+      <c r="D12">
+        <v>54.4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <v>57.2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>73.2</v>
+      </c>
+      <c r="D14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="32">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="D15">
+        <v>62.8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="D16">
+        <v>65.599999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>82.8</v>
+      </c>
+      <c r="D17">
+        <v>68.400000000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>86</v>
+      </c>
+      <c r="D18">
+        <v>71.2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>89.2</v>
+      </c>
+      <c r="D19">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>92.400000000000105</v>
+      </c>
+      <c r="D20" s="32">
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>95.600000000000094</v>
+      </c>
+      <c r="D21">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>98.800000000000097</v>
+      </c>
+      <c r="D22">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" s="32">
+        <v>102</v>
+      </c>
+      <c r="D23">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>105.2</v>
+      </c>
+      <c r="D24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>108.4</v>
+      </c>
+      <c r="D25">
+        <v>90.8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>111.6</v>
+      </c>
+      <c r="D26">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>114.8</v>
+      </c>
+      <c r="D27">
+        <v>96.4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>118</v>
+      </c>
+      <c r="D28">
+        <v>99.2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>121.2</v>
+      </c>
+      <c r="D29" s="32">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>124.4</v>
+      </c>
+      <c r="D30">
+        <v>104.8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" s="32">
+        <v>127.6</v>
+      </c>
+      <c r="D31">
+        <v>107.6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>130.80000000000001</v>
+      </c>
+      <c r="D32">
+        <v>110.4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>134</v>
+      </c>
+      <c r="D33">
+        <v>113.2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>137.19999999999999</v>
+      </c>
+      <c r="D34">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>140.4</v>
+      </c>
+      <c r="D35">
+        <v>118.8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>143.6</v>
+      </c>
+      <c r="D36">
+        <v>121.6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>146.80000000000001</v>
+      </c>
+      <c r="D37">
+        <v>124.4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" s="32">
+        <v>150</v>
+      </c>
+      <c r="D38" s="32">
+        <v>127.2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>153.19999999999999</v>
+      </c>
+      <c r="D39">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>156.4</v>
+      </c>
+      <c r="D40">
+        <v>132.80000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>159.6</v>
+      </c>
+      <c r="D41">
+        <v>135.6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>162.80000000000001</v>
+      </c>
+      <c r="D42">
+        <v>138.4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>166</v>
+      </c>
+      <c r="D43">
+        <v>141.19999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>169.2</v>
+      </c>
+      <c r="D44">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>172.4</v>
+      </c>
+      <c r="D45">
+        <v>146.80000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" s="32">
+        <v>175.6</v>
+      </c>
+      <c r="D46" s="32">
+        <v>149.6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>178.8</v>
+      </c>
+      <c r="D47">
+        <v>152.4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>182</v>
+      </c>
+      <c r="D48">
+        <v>155.19999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>185.2</v>
+      </c>
+      <c r="D49">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>188.4</v>
+      </c>
+      <c r="D50">
+        <v>160.80000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>191.6</v>
+      </c>
+      <c r="D51">
+        <v>163.6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>194.8</v>
+      </c>
+      <c r="D52">
+        <v>166.4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>198</v>
+      </c>
+      <c r="D53">
+        <v>169.2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54" s="32">
+        <v>201.2</v>
+      </c>
+      <c r="D54">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <v>204.4</v>
+      </c>
+      <c r="D55" s="32">
+        <v>174.8</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>207.6</v>
+      </c>
+      <c r="D56">
+        <v>177.6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <v>210.8</v>
+      </c>
+      <c r="D57">
+        <v>180.4</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <v>214</v>
+      </c>
+      <c r="D58">
+        <v>183.2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <v>217.2</v>
+      </c>
+      <c r="D59">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <v>220.4</v>
+      </c>
+      <c r="D60">
+        <v>188.8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <v>223.6</v>
+      </c>
+      <c r="D61">
+        <v>191.6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62" s="32">
+        <v>226.8</v>
+      </c>
+      <c r="D62">
+        <v>194.4</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <v>230</v>
+      </c>
+      <c r="D63">
+        <v>197.2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <v>233.2</v>
+      </c>
+      <c r="D64" s="32">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <v>236.4</v>
+      </c>
+      <c r="D65">
+        <v>202.8</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <v>239.6</v>
+      </c>
+      <c r="D66">
+        <v>205.6</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <v>242.8</v>
+      </c>
+      <c r="D67">
+        <v>208.4</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <v>246</v>
+      </c>
+      <c r="D68">
+        <v>211.2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <v>249.2</v>
+      </c>
+      <c r="D69">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70" s="32">
+        <v>252.4</v>
+      </c>
+      <c r="D70">
+        <v>216.8</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <v>255.6</v>
+      </c>
+      <c r="D71">
+        <v>219.6</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <v>258.8</v>
+      </c>
+      <c r="D72">
+        <v>222.4</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <v>262</v>
+      </c>
+      <c r="D73" s="32">
+        <v>225.2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <v>265.2</v>
+      </c>
+      <c r="D74">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <v>268.39999999999998</v>
+      </c>
+      <c r="D75">
+        <v>230.8</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76">
+        <v>271.60000000000002</v>
+      </c>
+      <c r="D76">
+        <v>233.6</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77" s="32">
+        <v>274.8</v>
+      </c>
+      <c r="D77">
+        <v>236.4</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <v>278</v>
+      </c>
+      <c r="D78">
+        <v>239.2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <v>281.2</v>
+      </c>
+      <c r="D79">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <v>284.39999999999998</v>
+      </c>
+      <c r="D80">
+        <v>244.8</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <v>287.60000000000002</v>
+      </c>
+      <c r="D81">
+        <v>247.6</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
+        <v>290.8</v>
+      </c>
+      <c r="D82" s="32">
+        <v>250.4</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83">
+        <v>294</v>
+      </c>
+      <c r="D83">
+        <v>253.2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
+        <v>297.2</v>
+      </c>
+      <c r="D84">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85" s="32">
+        <v>300.39999999999998</v>
+      </c>
+      <c r="D85">
+        <v>258.8</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86">
+        <v>303.60000000000002</v>
+      </c>
+      <c r="D86">
+        <v>261.60000000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87">
+        <v>306.8</v>
+      </c>
+      <c r="D87">
+        <v>264.39999999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <v>310</v>
+      </c>
+      <c r="D88">
+        <v>267.2</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89">
+        <v>313.2</v>
+      </c>
+      <c r="D89">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>89</v>
+      </c>
+      <c r="C90">
+        <v>316.39999999999998</v>
+      </c>
+      <c r="D90">
+        <v>272.8</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91">
+        <v>319.60000000000002</v>
+      </c>
+      <c r="D91" s="32">
+        <v>275.60000000000002</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92">
+        <v>322.8</v>
+      </c>
+      <c r="D92">
+        <v>278.39999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93" s="32">
+        <v>326</v>
+      </c>
+      <c r="D93">
+        <v>281.2</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <v>329.2</v>
+      </c>
+      <c r="D94">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95">
+        <v>332.4</v>
+      </c>
+      <c r="D95">
+        <v>286.8</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96">
+        <v>335.6</v>
+      </c>
+      <c r="D96">
+        <v>289.60000000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97">
+        <v>338.8</v>
+      </c>
+      <c r="D97">
+        <v>292.39999999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98">
+        <v>342</v>
+      </c>
+      <c r="D98">
+        <v>295.2</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99">
+        <v>345.2</v>
+      </c>
+      <c r="D99">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100">
+        <v>348.4</v>
+      </c>
+      <c r="D100" s="32">
+        <v>300.8</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101" s="32">
+        <v>351.6</v>
+      </c>
+      <c r="D101">
+        <v>303.60000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>101</v>
+      </c>
+      <c r="C102">
+        <v>354.8</v>
+      </c>
+      <c r="D102">
+        <v>306.39999999999998</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>102</v>
+      </c>
+      <c r="C103">
+        <v>358</v>
+      </c>
+      <c r="D103">
+        <v>309.2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>103</v>
+      </c>
+      <c r="C104">
+        <v>361.2</v>
+      </c>
+      <c r="D104">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>104</v>
+      </c>
+      <c r="C105">
+        <v>364.4</v>
+      </c>
+      <c r="D105">
+        <v>314.8</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>105</v>
+      </c>
+      <c r="C106">
+        <v>367.6</v>
+      </c>
+      <c r="D106">
+        <v>317.60000000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>106</v>
+      </c>
+      <c r="C107">
+        <v>370.8</v>
+      </c>
+      <c r="D107">
+        <v>320.39999999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>107</v>
+      </c>
+      <c r="C108">
+        <v>374</v>
+      </c>
+      <c r="D108">
+        <v>323.2</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>108</v>
+      </c>
+      <c r="C109" s="32">
+        <v>377.2</v>
+      </c>
+      <c r="D109" s="32">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>109</v>
+      </c>
+      <c r="C110">
+        <v>380.4</v>
+      </c>
+      <c r="D110">
+        <v>328.8</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>110</v>
+      </c>
+      <c r="C111">
+        <v>383.6</v>
+      </c>
+      <c r="D111">
+        <v>331.6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>111</v>
+      </c>
+      <c r="C112">
+        <v>386.8</v>
+      </c>
+      <c r="D112">
+        <v>334.4</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>112</v>
+      </c>
+      <c r="C113">
+        <v>390</v>
+      </c>
+      <c r="D113">
+        <v>337.2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>113</v>
+      </c>
+      <c r="C114">
+        <v>393.2</v>
+      </c>
+      <c r="D114">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>114</v>
+      </c>
+      <c r="C115">
+        <v>396.4</v>
+      </c>
+      <c r="D115">
+        <v>342.8</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>115</v>
+      </c>
+      <c r="C116" s="32">
+        <v>399.6</v>
+      </c>
+      <c r="D116">
+        <v>345.6</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>116</v>
+      </c>
+      <c r="C117">
+        <v>402.8</v>
+      </c>
+      <c r="D117">
+        <v>348.4</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>117</v>
+      </c>
+      <c r="C118">
+        <v>406</v>
+      </c>
+      <c r="D118" s="32">
+        <v>351.2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>118</v>
+      </c>
+      <c r="C119">
+        <v>409.2</v>
+      </c>
+      <c r="D119">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>119</v>
+      </c>
+      <c r="C120">
+        <v>412.4</v>
+      </c>
+      <c r="D120">
+        <v>356.8</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>120</v>
+      </c>
+      <c r="C121">
+        <v>415.6</v>
+      </c>
+      <c r="D121">
+        <v>359.6</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>121</v>
+      </c>
+      <c r="C122">
+        <v>418.8</v>
+      </c>
+      <c r="D122">
+        <v>362.4</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>122</v>
+      </c>
+      <c r="C123">
+        <v>422</v>
+      </c>
+      <c r="D123">
+        <v>365.2</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>123</v>
+      </c>
+      <c r="C124" s="32">
+        <v>425.2</v>
+      </c>
+      <c r="D124">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>124</v>
+      </c>
+      <c r="C125">
+        <v>428.4</v>
+      </c>
+      <c r="D125">
+        <v>370.8</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>125</v>
+      </c>
+      <c r="C126">
+        <v>431.6</v>
+      </c>
+      <c r="D126">
+        <v>373.6</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>126</v>
+      </c>
+      <c r="C127">
+        <v>434.8</v>
+      </c>
+      <c r="D127" s="32">
+        <v>376.4</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>127</v>
+      </c>
+      <c r="C128">
+        <v>438</v>
+      </c>
+      <c r="D128">
+        <v>379.2</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>128</v>
+      </c>
+      <c r="C129">
+        <v>441.2</v>
+      </c>
+      <c r="D129">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>129</v>
+      </c>
+      <c r="C130">
+        <v>444.4</v>
+      </c>
+      <c r="D130">
+        <v>384.8</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>130</v>
+      </c>
+      <c r="C131">
+        <v>447.6</v>
+      </c>
+      <c r="D131">
+        <v>387.6</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>131</v>
+      </c>
+      <c r="C132" s="32">
+        <v>450.8</v>
+      </c>
+      <c r="D132">
+        <v>390.4</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>132</v>
+      </c>
+      <c r="C133">
+        <v>454</v>
+      </c>
+      <c r="D133">
+        <v>393.2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>133</v>
+      </c>
+      <c r="C134">
+        <v>457.2</v>
+      </c>
+      <c r="D134">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>134</v>
+      </c>
+      <c r="C135">
+        <v>460.4</v>
+      </c>
+      <c r="D135" s="32">
+        <v>398.8</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>135</v>
+      </c>
+      <c r="C136">
+        <v>463.6</v>
+      </c>
+      <c r="D136">
+        <v>401.6</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>136</v>
+      </c>
+      <c r="C137">
+        <v>466.8</v>
+      </c>
+      <c r="D137">
+        <v>404.4</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>137</v>
+      </c>
+      <c r="C138">
+        <v>470</v>
+      </c>
+      <c r="D138">
+        <v>407.2</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>138</v>
+      </c>
+      <c r="C139">
+        <v>473.2</v>
+      </c>
+      <c r="D139">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>139</v>
+      </c>
+      <c r="C140" s="32">
+        <v>476.4</v>
+      </c>
+      <c r="D140">
+        <v>412.8</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>140</v>
+      </c>
+      <c r="C141">
+        <v>479.6</v>
+      </c>
+      <c r="D141">
+        <v>415.6</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>141</v>
+      </c>
+      <c r="C142">
+        <v>482.8</v>
+      </c>
+      <c r="D142">
+        <v>418.4</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>142</v>
+      </c>
+      <c r="C143">
+        <v>486</v>
+      </c>
+      <c r="D143">
+        <v>421.2</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>143</v>
+      </c>
+      <c r="C144">
+        <v>489.2</v>
+      </c>
+      <c r="D144">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>144</v>
+      </c>
+      <c r="C145">
+        <v>492.4</v>
+      </c>
+      <c r="D145" s="32">
+        <v>426.8</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>145</v>
+      </c>
+      <c r="C146">
+        <v>495.6</v>
+      </c>
+      <c r="D146">
+        <v>429.6</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>146</v>
+      </c>
+      <c r="C147" s="32">
+        <v>498.8</v>
+      </c>
+      <c r="D147">
+        <v>432.4</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>147</v>
+      </c>
+      <c r="C148">
+        <v>502</v>
+      </c>
+      <c r="D148">
+        <v>435.2</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>148</v>
+      </c>
+      <c r="C149">
+        <v>505.2</v>
+      </c>
+      <c r="D149">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>149</v>
+      </c>
+      <c r="C150">
+        <v>508.4</v>
+      </c>
+      <c r="D150">
+        <v>440.8</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>150</v>
+      </c>
+      <c r="C151">
+        <v>511.6</v>
+      </c>
+      <c r="D151">
+        <v>443.6</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>151</v>
+      </c>
+      <c r="C152">
+        <v>514.79999999999995</v>
+      </c>
+      <c r="D152">
+        <v>446.4</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>152</v>
+      </c>
+      <c r="C153">
+        <v>518</v>
+      </c>
+      <c r="D153" s="32">
+        <v>449.2</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>153</v>
+      </c>
+      <c r="C154">
+        <v>521.20000000000005</v>
+      </c>
+      <c r="D154">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>154</v>
+      </c>
+      <c r="C155">
+        <v>524.4</v>
+      </c>
+      <c r="D155">
+        <v>454.8</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>155</v>
+      </c>
+      <c r="C156">
+        <v>527.6</v>
+      </c>
+      <c r="D156">
+        <v>457.6</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>156</v>
+      </c>
+      <c r="C157">
+        <v>530.79999999999995</v>
+      </c>
+      <c r="D157">
+        <v>460.4</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>157</v>
+      </c>
+      <c r="C158">
+        <v>534</v>
+      </c>
+      <c r="D158">
+        <v>463.2</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>158</v>
+      </c>
+      <c r="C159">
+        <v>537.20000000000005</v>
+      </c>
+      <c r="D159">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>159</v>
+      </c>
+      <c r="C160">
+        <v>540.4</v>
+      </c>
+      <c r="D160">
+        <v>468.8</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>160</v>
+      </c>
+      <c r="C161">
+        <v>543.6</v>
+      </c>
+      <c r="D161">
+        <v>471.6</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>161</v>
+      </c>
+      <c r="C162">
+        <v>546.79999999999995</v>
+      </c>
+      <c r="D162">
+        <v>474.4</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>162</v>
+      </c>
+      <c r="C163">
+        <v>550.00000000000102</v>
+      </c>
+      <c r="D163" s="32">
+        <v>477.2</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>163</v>
+      </c>
+      <c r="C164">
+        <v>553.20000000000005</v>
+      </c>
+      <c r="D164">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>164</v>
+      </c>
+      <c r="C165">
+        <v>556.4</v>
+      </c>
+      <c r="D165">
+        <v>482.8</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>165</v>
+      </c>
+      <c r="C166">
+        <v>559.6</v>
+      </c>
+      <c r="D166">
+        <v>485.6</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>166</v>
+      </c>
+      <c r="C167">
+        <v>562.79999999999995</v>
+      </c>
+      <c r="D167">
+        <v>488.4</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>167</v>
+      </c>
+      <c r="C168">
+        <v>566.00000000000102</v>
+      </c>
+      <c r="D168">
+        <v>491.2</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>168</v>
+      </c>
+      <c r="C169">
+        <v>569.20000000000005</v>
+      </c>
+      <c r="D169">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>169</v>
+      </c>
+      <c r="C170">
+        <v>572.4</v>
+      </c>
+      <c r="D170">
+        <v>496.8</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>170</v>
+      </c>
+      <c r="C171">
+        <v>575.60000000000105</v>
+      </c>
+      <c r="D171" s="32">
+        <v>499.6</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>171</v>
+      </c>
+      <c r="C172">
+        <v>578.79999999999995</v>
+      </c>
+      <c r="D172">
+        <v>502.4</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>172</v>
+      </c>
+      <c r="C173">
+        <v>582.00000000000102</v>
+      </c>
+      <c r="D173">
+        <v>505.2</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>173</v>
+      </c>
+      <c r="C174">
+        <v>585.20000000000095</v>
+      </c>
+      <c r="D174">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>174</v>
+      </c>
+      <c r="C175">
+        <v>588.4</v>
+      </c>
+      <c r="D175">
+        <v>510.8</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>175</v>
+      </c>
+      <c r="C176">
+        <v>591.60000000000105</v>
+      </c>
+      <c r="D176">
+        <v>513.6</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>176</v>
+      </c>
+      <c r="C177">
+        <v>594.79999999999995</v>
+      </c>
+      <c r="D177">
+        <v>516.4</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>177</v>
+      </c>
+      <c r="C178">
+        <v>598.00000000000102</v>
+      </c>
+      <c r="D178">
+        <v>519.20000000000005</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>178</v>
+      </c>
+      <c r="C179">
+        <v>601.20000000000095</v>
+      </c>
+      <c r="D179">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>179</v>
+      </c>
+      <c r="C180">
+        <v>604.4</v>
+      </c>
+      <c r="D180">
+        <v>524.79999999999995</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>180</v>
+      </c>
+      <c r="C181">
+        <v>607.60000000000105</v>
+      </c>
+      <c r="D181">
+        <v>527.6</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>181</v>
+      </c>
+      <c r="C182">
+        <v>610.79999999999995</v>
+      </c>
+      <c r="D182">
+        <v>530.4</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>182</v>
+      </c>
+      <c r="C183">
+        <v>614.00000000000102</v>
+      </c>
+      <c r="D183">
+        <v>533.20000000000005</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>183</v>
+      </c>
+      <c r="C184">
+        <v>617.20000000000095</v>
+      </c>
+      <c r="D184">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>184</v>
+      </c>
+      <c r="C185">
+        <v>620.4</v>
+      </c>
+      <c r="D185">
+        <v>538.79999999999995</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>185</v>
+      </c>
+      <c r="C186">
+        <v>623.60000000000105</v>
+      </c>
+      <c r="D186">
+        <v>541.6</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>186</v>
+      </c>
+      <c r="C187">
+        <v>626.80000000000098</v>
+      </c>
+      <c r="D187">
+        <v>544.4</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>187</v>
+      </c>
+      <c r="C188">
+        <v>630.00000000000102</v>
+      </c>
+      <c r="D188">
+        <v>547.20000000000005</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>188</v>
+      </c>
+      <c r="C189">
+        <v>633.20000000000095</v>
+      </c>
+      <c r="D189">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>189</v>
+      </c>
+      <c r="C190">
+        <v>636.400000000001</v>
+      </c>
+      <c r="D190">
+        <v>552.79999999999995</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>190</v>
+      </c>
+      <c r="C191">
+        <v>639.60000000000105</v>
+      </c>
+      <c r="D191">
+        <v>555.6</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>191</v>
+      </c>
+      <c r="C192">
+        <v>642.80000000000098</v>
+      </c>
+      <c r="D192">
+        <v>558.4</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>192</v>
+      </c>
+      <c r="C193">
+        <v>646.00000000000102</v>
+      </c>
+      <c r="D193">
+        <v>561.20000000000005</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>193</v>
+      </c>
+      <c r="C194">
+        <v>649.20000000000095</v>
+      </c>
+      <c r="D194">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>194</v>
+      </c>
+      <c r="C195">
+        <v>652.400000000001</v>
+      </c>
+      <c r="D195">
+        <v>566.79999999999995</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>195</v>
+      </c>
+      <c r="C196">
+        <v>655.60000000000105</v>
+      </c>
+      <c r="D196">
+        <v>569.6</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>196</v>
+      </c>
+      <c r="C197">
+        <v>658.80000000000098</v>
+      </c>
+      <c r="D197">
+        <v>572.4</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>197</v>
+      </c>
+      <c r="C198">
+        <v>662.00000000000102</v>
+      </c>
+      <c r="D198">
+        <v>575.20000000000005</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>198</v>
+      </c>
+      <c r="C199">
+        <v>665.20000000000095</v>
+      </c>
+      <c r="D199">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>199</v>
+      </c>
+      <c r="C200">
+        <v>668.400000000001</v>
+      </c>
+      <c r="D200">
+        <v>580.79999999999995</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>200</v>
+      </c>
+      <c r="C201">
+        <v>671.60000000000105</v>
+      </c>
+      <c r="D201">
+        <v>583.6</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>201</v>
+      </c>
+      <c r="C202">
+        <v>674.80000000000098</v>
+      </c>
+      <c r="D202">
+        <v>586.4</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <v>202</v>
+      </c>
+      <c r="C203">
+        <v>678.00000000000102</v>
+      </c>
+      <c r="D203">
+        <v>589.20000000000005</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>203</v>
+      </c>
+      <c r="C204">
+        <v>681.20000000000095</v>
+      </c>
+      <c r="D204">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>204</v>
+      </c>
+      <c r="C205">
+        <v>684.400000000001</v>
+      </c>
+      <c r="D205">
+        <v>594.79999999999995</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>205</v>
+      </c>
+      <c r="C206">
+        <v>687.60000000000105</v>
+      </c>
+      <c r="D206">
+        <v>597.6</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <v>206</v>
+      </c>
+      <c r="C207">
+        <v>690.80000000000098</v>
+      </c>
+      <c r="D207">
+        <v>600.4</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>207</v>
+      </c>
+      <c r="C208">
+        <v>694.00000000000102</v>
+      </c>
+      <c r="D208">
+        <v>603.20000000000005</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>208</v>
+      </c>
+      <c r="C209">
+        <v>697.20000000000095</v>
+      </c>
+      <c r="D209">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>209</v>
+      </c>
+      <c r="C210">
+        <v>700.400000000001</v>
+      </c>
+      <c r="D210">
+        <v>608.79999999999995</v>
+      </c>
+    </row>
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>210</v>
+      </c>
+      <c r="C211">
+        <v>703.60000000000105</v>
+      </c>
+      <c r="D211">
+        <v>611.6</v>
+      </c>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>211</v>
+      </c>
+      <c r="C212">
+        <v>706.80000000000098</v>
+      </c>
+      <c r="D212">
+        <v>614.4</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>212</v>
+      </c>
+      <c r="C213">
+        <v>710.00000000000102</v>
+      </c>
+      <c r="D213">
+        <v>617.20000000000005</v>
+      </c>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>213</v>
+      </c>
+      <c r="C214">
+        <v>713.20000000000095</v>
+      </c>
+      <c r="D214">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>214</v>
+      </c>
+      <c r="C215">
+        <v>716.400000000001</v>
+      </c>
+      <c r="D215">
+        <v>622.79999999999995</v>
+      </c>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>215</v>
+      </c>
+      <c r="C216">
+        <v>719.60000000000105</v>
+      </c>
+      <c r="D216">
+        <v>625.6</v>
+      </c>
+    </row>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>216</v>
+      </c>
+      <c r="C217">
+        <v>722.80000000000098</v>
+      </c>
+      <c r="D217">
+        <v>628.4</v>
+      </c>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>217</v>
+      </c>
+      <c r="C218">
+        <v>726.00000000000102</v>
+      </c>
+      <c r="D218">
+        <v>631.20000000000005</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <v>218</v>
+      </c>
+      <c r="C219">
+        <v>729.20000000000095</v>
+      </c>
+      <c r="D219">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>219</v>
+      </c>
+      <c r="C220">
+        <v>732.400000000001</v>
+      </c>
+      <c r="D220">
+        <v>636.79999999999995</v>
+      </c>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>220</v>
+      </c>
+      <c r="C221">
+        <v>735.60000000000105</v>
+      </c>
+      <c r="D221">
+        <v>639.6</v>
+      </c>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>221</v>
+      </c>
+      <c r="C222">
+        <v>738.80000000000098</v>
+      </c>
+      <c r="D222">
+        <v>642.4</v>
+      </c>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>222</v>
+      </c>
+      <c r="C223">
+        <v>742.00000000000102</v>
+      </c>
+      <c r="D223">
+        <v>645.20000000000005</v>
+      </c>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>223</v>
+      </c>
+      <c r="C224">
+        <v>745.20000000000095</v>
+      </c>
+      <c r="D224">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>224</v>
+      </c>
+      <c r="C225">
+        <v>748.400000000001</v>
+      </c>
+      <c r="D225">
+        <v>650.79999999999995</v>
+      </c>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>225</v>
+      </c>
+      <c r="C226">
+        <v>751.60000000000105</v>
+      </c>
+      <c r="D226">
+        <v>653.6</v>
+      </c>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <v>226</v>
+      </c>
+      <c r="C227">
+        <v>754.80000000000098</v>
+      </c>
+      <c r="D227">
+        <v>656.4</v>
+      </c>
+    </row>
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <v>227</v>
+      </c>
+      <c r="C228">
+        <v>758.00000000000102</v>
+      </c>
+      <c r="D228">
+        <v>659.2</v>
+      </c>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <v>228</v>
+      </c>
+      <c r="C229">
+        <v>761.20000000000095</v>
+      </c>
+      <c r="D229">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <v>229</v>
+      </c>
+      <c r="C230">
+        <v>764.400000000001</v>
+      </c>
+      <c r="D230">
+        <v>664.8</v>
+      </c>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <v>230</v>
+      </c>
+      <c r="C231">
+        <v>767.60000000000105</v>
+      </c>
+      <c r="D231">
+        <v>667.6</v>
+      </c>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B232">
+        <v>231</v>
+      </c>
+      <c r="C232">
+        <v>770.80000000000098</v>
+      </c>
+      <c r="D232">
+        <v>670.4</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>232</v>
+      </c>
+      <c r="C233">
+        <v>774.00000000000102</v>
+      </c>
+      <c r="D233">
+        <v>673.2</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>233</v>
+      </c>
+      <c r="C234">
+        <v>777.20000000000095</v>
+      </c>
+      <c r="D234">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>234</v>
+      </c>
+      <c r="C235">
+        <v>780.400000000001</v>
+      </c>
+      <c r="D235">
+        <v>678.8</v>
+      </c>
+    </row>
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>235</v>
+      </c>
+      <c r="C236">
+        <v>783.60000000000105</v>
+      </c>
+      <c r="D236">
+        <v>681.6</v>
+      </c>
+    </row>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>236</v>
+      </c>
+      <c r="C237">
+        <v>786.80000000000098</v>
+      </c>
+      <c r="D237">
+        <v>684.4</v>
+      </c>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>237</v>
+      </c>
+      <c r="C238">
+        <v>790.00000000000102</v>
+      </c>
+      <c r="D238">
+        <v>687.2</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>238</v>
+      </c>
+      <c r="C239">
+        <v>793.20000000000095</v>
+      </c>
+      <c r="D239">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>239</v>
+      </c>
+      <c r="C240">
+        <v>796.400000000001</v>
+      </c>
+      <c r="D240">
+        <v>692.8</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>240</v>
+      </c>
+      <c r="C241">
+        <v>799.60000000000105</v>
+      </c>
+      <c r="D241">
+        <v>695.6</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>241</v>
+      </c>
+      <c r="C242">
+        <v>802.80000000000098</v>
+      </c>
+      <c r="D242">
+        <v>698.4</v>
+      </c>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>242</v>
+      </c>
+      <c r="C243">
+        <v>806.00000000000102</v>
+      </c>
+      <c r="D243">
+        <v>701.2</v>
+      </c>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>243</v>
+      </c>
+      <c r="C244">
+        <v>809.20000000000095</v>
+      </c>
+      <c r="D244">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <v>244</v>
+      </c>
+      <c r="C245">
+        <v>812.400000000001</v>
+      </c>
+      <c r="D245">
+        <v>706.8</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <v>245</v>
+      </c>
+      <c r="C246">
+        <v>815.60000000000105</v>
+      </c>
+      <c r="D246">
+        <v>709.6</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>246</v>
+      </c>
+      <c r="C247">
+        <v>818.80000000000098</v>
+      </c>
+      <c r="D247">
+        <v>712.4</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>247</v>
+      </c>
+      <c r="C248">
+        <v>822.00000000000102</v>
+      </c>
+      <c r="D248">
+        <v>715.2</v>
+      </c>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <v>248</v>
+      </c>
+      <c r="C249">
+        <v>825.20000000000095</v>
+      </c>
+      <c r="D249">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>249</v>
+      </c>
+      <c r="C250">
+        <v>828.400000000001</v>
+      </c>
+      <c r="D250">
+        <v>720.8</v>
+      </c>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>250</v>
+      </c>
+      <c r="C251">
+        <v>831.60000000000105</v>
+      </c>
+      <c r="D251">
+        <v>723.6</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>251</v>
+      </c>
+      <c r="C252">
+        <v>834.80000000000098</v>
+      </c>
+      <c r="D252">
+        <v>726.4</v>
+      </c>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>252</v>
+      </c>
+      <c r="C253">
+        <v>838.00000000000102</v>
+      </c>
+      <c r="D253">
+        <v>729.2</v>
+      </c>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>253</v>
+      </c>
+      <c r="C254">
+        <v>841.20000000000095</v>
+      </c>
+      <c r="D254">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>254</v>
+      </c>
+      <c r="C255">
+        <v>844.400000000001</v>
+      </c>
+      <c r="D255">
+        <v>734.8</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <v>255</v>
+      </c>
+      <c r="C256">
+        <v>847.60000000000105</v>
+      </c>
+      <c r="D256">
+        <v>737.6</v>
+      </c>
+    </row>
+    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <v>256</v>
+      </c>
+      <c r="C257">
+        <v>850.80000000000098</v>
+      </c>
+      <c r="D257">
+        <v>740.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up repo a bit: remove temp files from tracking
</commit_message>
<xml_diff>
--- a/HeadArray/HA_HHP_HeadArrayTimingAnalysis.xlsx
+++ b/HeadArray/HA_HHP_HeadArrayTimingAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Invacare\ASL110\ASL110_Documentation\HeadArray\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2965D2E-72B4-416E-ADC9-735EF1FD3512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFDBC55-5516-4635-BA34-A2D3C7737F1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{1CC3B75C-6B58-4B8C-B05F-04D899897821}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{1CC3B75C-6B58-4B8C-B05F-04D899897821}"/>
   </bookViews>
   <sheets>
     <sheet name="SingleFunc" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
   <si>
     <t>Optimization 2 (w/ or w/o focus on Debug)</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Optimization 2 (Measured)</t>
+  </si>
+  <si>
+    <t>Actual (us)</t>
   </si>
 </sst>
 </file>
@@ -487,28 +490,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -523,7 +506,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,16 +858,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="E2" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="E2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1059,44 +1062,44 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="31"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="25"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="15"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="21" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="21" t="s">
+      <c r="J3" s="27"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="23"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -1435,44 +1438,44 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="31"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="25"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="21" t="s">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="21" t="s">
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="21" t="s">
+      <c r="J13" s="27"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="27"/>
-      <c r="N13" s="23"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="28"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
@@ -1802,10 +1805,10 @@
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="21"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
@@ -1824,10 +1827,10 @@
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="20"/>
+      <c r="C28" s="21"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
@@ -1844,6 +1847,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="B2:N2"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B12:N12"/>
@@ -1851,11 +1859,6 @@
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="L13:N13"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="B2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1873,10 +1876,10 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C1" s="2"/>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="20"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -5215,10 +5218,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9918BCC6-78DB-4BFB-93F8-A53989EA45CB}">
-  <dimension ref="A3:K15"/>
+  <dimension ref="A3:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H6"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5228,25 +5231,29 @@
     <col min="3" max="3" width="3.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D3" s="20" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
@@ -5254,33 +5261,47 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
         <v>34.799999999999997</v>
       </c>
-      <c r="G5">
+      <c r="F5">
+        <f>E5-$A$11</f>
+        <v>17.199999999999996</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>26.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f>I5-$A$15</f>
+        <v>11.599999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>2</v>
       </c>
@@ -5288,25 +5309,33 @@
         <v>38</v>
       </c>
       <c r="F6">
+        <f t="shared" ref="F6:F14" si="0">E6-$A$11</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="G6">
         <f>E6-E5</f>
         <v>3.2000000000000028</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>29.2</v>
       </c>
-      <c r="I6">
-        <f>H6-H5</f>
+      <c r="J6">
+        <f t="shared" ref="J6:J14" si="1">I6-$A$15</f>
+        <v>14.399999999999999</v>
+      </c>
+      <c r="K6">
+        <f>I6-I5</f>
         <v>2.8000000000000007</v>
       </c>
-      <c r="K6">
-        <f>AVERAGE(I6:I9)</f>
+      <c r="M6">
+        <f>AVERAGE(K6:K9)</f>
         <v>2.8000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>3</v>
       </c>
@@ -5314,21 +5343,29 @@
         <v>41.2</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F10" si="0">E7-E6</f>
+        <f t="shared" si="0"/>
+        <v>23.6</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G9" si="2">E7-E6</f>
         <v>3.2000000000000028</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>3</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>32</v>
       </c>
-      <c r="I7">
-        <f t="shared" ref="I7:I10" si="1">H7-H6</f>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>17.2</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K9" si="3">I7-I6</f>
         <v>2.8000000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>4</v>
       </c>
@@ -5337,24 +5374,32 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
+        <v>26.799999999999997</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
         <v>3.1999999999999957</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>4</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>34.9</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>20.099999999999998</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
         <v>2.8999999999999986</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="21"/>
       <c r="D9">
         <v>5</v>
       </c>
@@ -5363,20 +5408,28 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
         <v>3.2000000000000028</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>5</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>37.6</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>22.8</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
         <v>2.7000000000000028</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -5386,14 +5439,22 @@
       <c r="E10">
         <v>2098.1</v>
       </c>
-      <c r="G10">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2080.5</v>
+      </c>
+      <c r="H10">
         <v>256</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>2001.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>1986.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>17.600000000000001</v>
       </c>
@@ -5407,25 +5468,33 @@
         <v>2107.4</v>
       </c>
       <c r="F11">
+        <f t="shared" si="0"/>
+        <v>2089.8000000000002</v>
+      </c>
+      <c r="G11">
         <f>E11-E10</f>
         <v>9.3000000000001819</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>257</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>2010.6</v>
       </c>
-      <c r="I11">
-        <f>H11-H10</f>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>1995.8</v>
+      </c>
+      <c r="K11">
+        <f>I11-I10</f>
         <v>8.8999999999998636</v>
       </c>
-      <c r="K11">
-        <f>AVERAGE(I11:I14)</f>
+      <c r="M11">
+        <f>AVERAGE(K11:K14)</f>
         <v>8.8000000000000114</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="D12">
         <v>258</v>
@@ -5434,25 +5503,33 @@
         <v>2116.5</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F14" si="2">E12-E11</f>
+        <f t="shared" si="0"/>
+        <v>2098.9</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G14" si="4">E12-E11</f>
         <v>9.0999999999999091</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>258</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>2019.3</v>
       </c>
-      <c r="I12">
-        <f t="shared" ref="I12:I14" si="3">H12-H11</f>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>2004.5</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K12:K14" si="5">I12-I11</f>
         <v>8.7000000000000455</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="20"/>
+      <c r="B13" s="21"/>
       <c r="D13">
         <v>259</v>
       </c>
@@ -5460,21 +5537,29 @@
         <v>2125.8000000000002</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>2108.2000000000003</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
         <v>9.3000000000001819</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>259</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>2028.2</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="3"/>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>2013.4</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="5"/>
         <v>8.9000000000000909</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -5485,21 +5570,29 @@
         <v>2134.9</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>2117.3000000000002</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
         <v>9.0999999999999091</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>260</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>2036.9</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="3"/>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>2022.1000000000001</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="5"/>
         <v>8.7000000000000455</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14.8</v>
       </c>
@@ -5511,8 +5604,8 @@
   <mergeCells count="4">
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="D3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5523,7 +5616,7 @@
   <dimension ref="B1:D257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D163" activeCellId="1" sqref="C140 D163"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5540,11 +5633,11 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="32">
-        <v>34.799999999999997</v>
+      <c r="C2" s="20">
+        <v>16.399999999999999</v>
       </c>
       <c r="D2">
-        <v>26.4</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -5552,10 +5645,12 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>38</v>
+        <f>C2+3.2</f>
+        <v>19.599999999999998</v>
       </c>
       <c r="D3">
-        <v>29.2</v>
+        <f>D2+2.8</f>
+        <v>14.399999999999999</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -5563,10 +5658,12 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>41.2</v>
+        <f t="shared" ref="C4:C67" si="0">C3+3.2</f>
+        <v>22.799999999999997</v>
       </c>
       <c r="D4">
-        <v>32</v>
+        <f t="shared" ref="D4:D67" si="1">D3+2.8</f>
+        <v>17.2</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -5574,10 +5671,12 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>44.4</v>
-      </c>
-      <c r="D5" s="32">
-        <v>34.799999999999997</v>
+        <f t="shared" si="0"/>
+        <v>25.999999999999996</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -5585,21 +5684,25 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>47.6</v>
+        <f t="shared" si="0"/>
+        <v>29.199999999999996</v>
       </c>
       <c r="D6">
-        <v>37.6</v>
+        <f t="shared" si="1"/>
+        <v>22.8</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="32">
-        <v>50.8</v>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>32.4</v>
       </c>
       <c r="D7">
-        <v>40.4</v>
+        <f t="shared" si="1"/>
+        <v>25.6</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -5607,10 +5710,12 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>54</v>
+        <f t="shared" si="0"/>
+        <v>35.6</v>
       </c>
       <c r="D8">
-        <v>43.2</v>
+        <f t="shared" si="1"/>
+        <v>28.400000000000002</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -5618,10 +5723,12 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>57.2</v>
+        <f t="shared" si="0"/>
+        <v>38.800000000000004</v>
       </c>
       <c r="D9">
-        <v>46</v>
+        <f t="shared" si="1"/>
+        <v>31.200000000000003</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -5629,10 +5736,12 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>60.4</v>
+        <f t="shared" si="0"/>
+        <v>42.000000000000007</v>
       </c>
       <c r="D10">
-        <v>48.8</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -5640,10 +5749,12 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>63.6</v>
-      </c>
-      <c r="D11" s="32">
-        <v>51.6</v>
+        <f t="shared" si="0"/>
+        <v>45.20000000000001</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>36.799999999999997</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -5651,10 +5762,12 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>66.8</v>
+        <f t="shared" si="0"/>
+        <v>48.400000000000013</v>
       </c>
       <c r="D12">
-        <v>54.4</v>
+        <f t="shared" si="1"/>
+        <v>39.599999999999994</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -5662,10 +5775,12 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>70</v>
+        <f t="shared" si="0"/>
+        <v>51.600000000000016</v>
       </c>
       <c r="D13">
-        <v>57.2</v>
+        <f t="shared" si="1"/>
+        <v>42.399999999999991</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -5673,21 +5788,25 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>73.2</v>
+        <f t="shared" si="0"/>
+        <v>54.800000000000018</v>
       </c>
       <c r="D14">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>45.199999999999989</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="32">
-        <v>76.400000000000006</v>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>58.000000000000021</v>
       </c>
       <c r="D15">
-        <v>62.8</v>
+        <f t="shared" si="1"/>
+        <v>47.999999999999986</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
@@ -5695,10 +5814,12 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>79.599999999999994</v>
+        <f t="shared" si="0"/>
+        <v>61.200000000000024</v>
       </c>
       <c r="D16">
-        <v>65.599999999999994</v>
+        <f t="shared" si="1"/>
+        <v>50.799999999999983</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -5706,10 +5827,12 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>82.8</v>
+        <f t="shared" si="0"/>
+        <v>64.40000000000002</v>
       </c>
       <c r="D17">
-        <v>68.400000000000006</v>
+        <f t="shared" si="1"/>
+        <v>53.59999999999998</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -5717,10 +5840,12 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>86</v>
+        <f t="shared" si="0"/>
+        <v>67.600000000000023</v>
       </c>
       <c r="D18">
-        <v>71.2</v>
+        <f t="shared" si="1"/>
+        <v>56.399999999999977</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -5728,10 +5853,12 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>89.2</v>
+        <f t="shared" si="0"/>
+        <v>70.800000000000026</v>
       </c>
       <c r="D19">
-        <v>74</v>
+        <f t="shared" si="1"/>
+        <v>59.199999999999974</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -5739,10 +5866,12 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <v>92.400000000000105</v>
-      </c>
-      <c r="D20" s="32">
-        <v>76.8</v>
+        <f t="shared" si="0"/>
+        <v>74.000000000000028</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>61.999999999999972</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -5750,10 +5879,12 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>95.600000000000094</v>
+        <f t="shared" si="0"/>
+        <v>77.200000000000031</v>
       </c>
       <c r="D21">
-        <v>79.599999999999994</v>
+        <f t="shared" si="1"/>
+        <v>64.799999999999969</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -5761,21 +5892,25 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <v>98.800000000000097</v>
+        <f t="shared" si="0"/>
+        <v>80.400000000000034</v>
       </c>
       <c r="D22">
-        <v>82.4</v>
+        <f t="shared" si="1"/>
+        <v>67.599999999999966</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>22</v>
       </c>
-      <c r="C23" s="32">
-        <v>102</v>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>83.600000000000037</v>
       </c>
       <c r="D23">
-        <v>85.2</v>
+        <f t="shared" si="1"/>
+        <v>70.399999999999963</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -5783,10 +5918,12 @@
         <v>23</v>
       </c>
       <c r="C24">
-        <v>105.2</v>
+        <f t="shared" si="0"/>
+        <v>86.80000000000004</v>
       </c>
       <c r="D24">
-        <v>88</v>
+        <f t="shared" si="1"/>
+        <v>73.19999999999996</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -5794,10 +5931,12 @@
         <v>24</v>
       </c>
       <c r="C25">
-        <v>108.4</v>
+        <f t="shared" si="0"/>
+        <v>90.000000000000043</v>
       </c>
       <c r="D25">
-        <v>90.8</v>
+        <f t="shared" si="1"/>
+        <v>75.999999999999957</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -5805,10 +5944,12 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>111.6</v>
+        <f t="shared" si="0"/>
+        <v>93.200000000000045</v>
       </c>
       <c r="D26">
-        <v>93.6</v>
+        <f t="shared" si="1"/>
+        <v>78.799999999999955</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -5816,10 +5957,12 @@
         <v>26</v>
       </c>
       <c r="C27">
-        <v>114.8</v>
+        <f t="shared" si="0"/>
+        <v>96.400000000000048</v>
       </c>
       <c r="D27">
-        <v>96.4</v>
+        <f t="shared" si="1"/>
+        <v>81.599999999999952</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -5827,10 +5970,12 @@
         <v>27</v>
       </c>
       <c r="C28">
-        <v>118</v>
+        <f t="shared" si="0"/>
+        <v>99.600000000000051</v>
       </c>
       <c r="D28">
-        <v>99.2</v>
+        <f t="shared" si="1"/>
+        <v>84.399999999999949</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -5838,10 +5983,12 @@
         <v>28</v>
       </c>
       <c r="C29">
-        <v>121.2</v>
-      </c>
-      <c r="D29" s="32">
-        <v>102</v>
+        <f t="shared" si="0"/>
+        <v>102.80000000000005</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>87.199999999999946</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -5849,21 +5996,25 @@
         <v>29</v>
       </c>
       <c r="C30">
-        <v>124.4</v>
+        <f t="shared" si="0"/>
+        <v>106.00000000000006</v>
       </c>
       <c r="D30">
-        <v>104.8</v>
+        <f t="shared" si="1"/>
+        <v>89.999999999999943</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>30</v>
       </c>
-      <c r="C31" s="32">
-        <v>127.6</v>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>109.20000000000006</v>
       </c>
       <c r="D31">
-        <v>107.6</v>
+        <f t="shared" si="1"/>
+        <v>92.79999999999994</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -5871,10 +6022,12 @@
         <v>31</v>
       </c>
       <c r="C32">
-        <v>130.80000000000001</v>
+        <f t="shared" si="0"/>
+        <v>112.40000000000006</v>
       </c>
       <c r="D32">
-        <v>110.4</v>
+        <f t="shared" si="1"/>
+        <v>95.599999999999937</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -5882,10 +6035,12 @@
         <v>32</v>
       </c>
       <c r="C33">
-        <v>134</v>
+        <f t="shared" si="0"/>
+        <v>115.60000000000007</v>
       </c>
       <c r="D33">
-        <v>113.2</v>
+        <f t="shared" si="1"/>
+        <v>98.399999999999935</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -5893,10 +6048,12 @@
         <v>33</v>
       </c>
       <c r="C34">
-        <v>137.19999999999999</v>
+        <f t="shared" si="0"/>
+        <v>118.80000000000007</v>
       </c>
       <c r="D34">
-        <v>116</v>
+        <f t="shared" si="1"/>
+        <v>101.19999999999993</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -5904,10 +6061,12 @@
         <v>34</v>
       </c>
       <c r="C35">
-        <v>140.4</v>
+        <f t="shared" si="0"/>
+        <v>122.00000000000007</v>
       </c>
       <c r="D35">
-        <v>118.8</v>
+        <f t="shared" si="1"/>
+        <v>103.99999999999993</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -5915,10 +6074,12 @@
         <v>35</v>
       </c>
       <c r="C36">
-        <v>143.6</v>
+        <f t="shared" si="0"/>
+        <v>125.20000000000007</v>
       </c>
       <c r="D36">
-        <v>121.6</v>
+        <f t="shared" si="1"/>
+        <v>106.79999999999993</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
@@ -5926,21 +6087,25 @@
         <v>36</v>
       </c>
       <c r="C37">
-        <v>146.80000000000001</v>
+        <f t="shared" si="0"/>
+        <v>128.40000000000006</v>
       </c>
       <c r="D37">
-        <v>124.4</v>
+        <f t="shared" si="1"/>
+        <v>109.59999999999992</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>37</v>
       </c>
-      <c r="C38" s="32">
-        <v>150</v>
-      </c>
-      <c r="D38" s="32">
-        <v>127.2</v>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>131.60000000000005</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>112.39999999999992</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -5948,10 +6113,12 @@
         <v>38</v>
       </c>
       <c r="C39">
-        <v>153.19999999999999</v>
+        <f t="shared" si="0"/>
+        <v>134.80000000000004</v>
       </c>
       <c r="D39">
-        <v>130</v>
+        <f t="shared" si="1"/>
+        <v>115.19999999999992</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -5959,10 +6126,12 @@
         <v>39</v>
       </c>
       <c r="C40">
-        <v>156.4</v>
+        <f t="shared" si="0"/>
+        <v>138.00000000000003</v>
       </c>
       <c r="D40">
-        <v>132.80000000000001</v>
+        <f t="shared" si="1"/>
+        <v>117.99999999999991</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -5970,10 +6139,12 @@
         <v>40</v>
       </c>
       <c r="C41">
-        <v>159.6</v>
+        <f t="shared" si="0"/>
+        <v>141.20000000000002</v>
       </c>
       <c r="D41">
-        <v>135.6</v>
+        <f t="shared" si="1"/>
+        <v>120.79999999999991</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
@@ -5981,10 +6152,12 @@
         <v>41</v>
       </c>
       <c r="C42">
-        <v>162.80000000000001</v>
+        <f t="shared" si="0"/>
+        <v>144.4</v>
       </c>
       <c r="D42">
-        <v>138.4</v>
+        <f t="shared" si="1"/>
+        <v>123.59999999999991</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -5992,10 +6165,12 @@
         <v>42</v>
       </c>
       <c r="C43">
-        <v>166</v>
+        <f t="shared" si="0"/>
+        <v>147.6</v>
       </c>
       <c r="D43">
-        <v>141.19999999999999</v>
+        <f t="shared" si="1"/>
+        <v>126.39999999999991</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
@@ -6003,10 +6178,12 @@
         <v>43</v>
       </c>
       <c r="C44">
-        <v>169.2</v>
+        <f t="shared" si="0"/>
+        <v>150.79999999999998</v>
       </c>
       <c r="D44">
-        <v>144</v>
+        <f t="shared" si="1"/>
+        <v>129.1999999999999</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
@@ -6014,21 +6191,25 @@
         <v>44</v>
       </c>
       <c r="C45">
-        <v>172.4</v>
+        <f t="shared" si="0"/>
+        <v>153.99999999999997</v>
       </c>
       <c r="D45">
-        <v>146.80000000000001</v>
+        <f t="shared" si="1"/>
+        <v>131.99999999999991</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>45</v>
       </c>
-      <c r="C46" s="32">
-        <v>175.6</v>
-      </c>
-      <c r="D46" s="32">
-        <v>149.6</v>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>157.19999999999996</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>134.79999999999993</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
@@ -6036,10 +6217,12 @@
         <v>46</v>
       </c>
       <c r="C47">
-        <v>178.8</v>
+        <f t="shared" si="0"/>
+        <v>160.39999999999995</v>
       </c>
       <c r="D47">
-        <v>152.4</v>
+        <f t="shared" si="1"/>
+        <v>137.59999999999994</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
@@ -6047,10 +6230,12 @@
         <v>47</v>
       </c>
       <c r="C48">
-        <v>182</v>
+        <f t="shared" si="0"/>
+        <v>163.59999999999994</v>
       </c>
       <c r="D48">
-        <v>155.19999999999999</v>
+        <f t="shared" si="1"/>
+        <v>140.39999999999995</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
@@ -6058,10 +6243,12 @@
         <v>48</v>
       </c>
       <c r="C49">
-        <v>185.2</v>
+        <f t="shared" si="0"/>
+        <v>166.79999999999993</v>
       </c>
       <c r="D49">
-        <v>158</v>
+        <f t="shared" si="1"/>
+        <v>143.19999999999996</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
@@ -6069,10 +6256,12 @@
         <v>49</v>
       </c>
       <c r="C50">
-        <v>188.4</v>
+        <f t="shared" si="0"/>
+        <v>169.99999999999991</v>
       </c>
       <c r="D50">
-        <v>160.80000000000001</v>
+        <f t="shared" si="1"/>
+        <v>145.99999999999997</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
@@ -6080,10 +6269,12 @@
         <v>50</v>
       </c>
       <c r="C51">
-        <v>191.6</v>
+        <f t="shared" si="0"/>
+        <v>173.1999999999999</v>
       </c>
       <c r="D51">
-        <v>163.6</v>
+        <f t="shared" si="1"/>
+        <v>148.79999999999998</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
@@ -6091,10 +6282,12 @@
         <v>51</v>
       </c>
       <c r="C52">
-        <v>194.8</v>
+        <f t="shared" si="0"/>
+        <v>176.39999999999989</v>
       </c>
       <c r="D52">
-        <v>166.4</v>
+        <f t="shared" si="1"/>
+        <v>151.6</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
@@ -6102,21 +6295,25 @@
         <v>52</v>
       </c>
       <c r="C53">
-        <v>198</v>
+        <f t="shared" si="0"/>
+        <v>179.59999999999988</v>
       </c>
       <c r="D53">
-        <v>169.2</v>
+        <f t="shared" si="1"/>
+        <v>154.4</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>53</v>
       </c>
-      <c r="C54" s="32">
-        <v>201.2</v>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>182.79999999999987</v>
       </c>
       <c r="D54">
-        <v>172</v>
+        <f t="shared" si="1"/>
+        <v>157.20000000000002</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
@@ -6124,10 +6321,12 @@
         <v>54</v>
       </c>
       <c r="C55">
-        <v>204.4</v>
-      </c>
-      <c r="D55" s="32">
-        <v>174.8</v>
+        <f t="shared" si="0"/>
+        <v>185.99999999999986</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>160.00000000000003</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
@@ -6135,10 +6334,12 @@
         <v>55</v>
       </c>
       <c r="C56">
-        <v>207.6</v>
+        <f t="shared" si="0"/>
+        <v>189.19999999999985</v>
       </c>
       <c r="D56">
-        <v>177.6</v>
+        <f t="shared" si="1"/>
+        <v>162.80000000000004</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
@@ -6146,10 +6347,12 @@
         <v>56</v>
       </c>
       <c r="C57">
-        <v>210.8</v>
+        <f t="shared" si="0"/>
+        <v>192.39999999999984</v>
       </c>
       <c r="D57">
-        <v>180.4</v>
+        <f t="shared" si="1"/>
+        <v>165.60000000000005</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
@@ -6157,10 +6360,12 @@
         <v>57</v>
       </c>
       <c r="C58">
-        <v>214</v>
+        <f t="shared" si="0"/>
+        <v>195.59999999999982</v>
       </c>
       <c r="D58">
-        <v>183.2</v>
+        <f t="shared" si="1"/>
+        <v>168.40000000000006</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
@@ -6168,10 +6373,12 @@
         <v>58</v>
       </c>
       <c r="C59">
-        <v>217.2</v>
+        <f t="shared" si="0"/>
+        <v>198.79999999999981</v>
       </c>
       <c r="D59">
-        <v>186</v>
+        <f t="shared" si="1"/>
+        <v>171.20000000000007</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
@@ -6179,10 +6386,12 @@
         <v>59</v>
       </c>
       <c r="C60">
-        <v>220.4</v>
+        <f t="shared" si="0"/>
+        <v>201.9999999999998</v>
       </c>
       <c r="D60">
-        <v>188.8</v>
+        <f t="shared" si="1"/>
+        <v>174.00000000000009</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
@@ -6190,21 +6399,25 @@
         <v>60</v>
       </c>
       <c r="C61">
-        <v>223.6</v>
+        <f t="shared" si="0"/>
+        <v>205.19999999999979</v>
       </c>
       <c r="D61">
-        <v>191.6</v>
+        <f t="shared" si="1"/>
+        <v>176.8000000000001</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>61</v>
       </c>
-      <c r="C62" s="32">
-        <v>226.8</v>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>208.39999999999978</v>
       </c>
       <c r="D62">
-        <v>194.4</v>
+        <f t="shared" si="1"/>
+        <v>179.60000000000011</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
@@ -6212,10 +6425,12 @@
         <v>62</v>
       </c>
       <c r="C63">
-        <v>230</v>
+        <f t="shared" si="0"/>
+        <v>211.59999999999977</v>
       </c>
       <c r="D63">
-        <v>197.2</v>
+        <f t="shared" si="1"/>
+        <v>182.40000000000012</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
@@ -6223,10 +6438,12 @@
         <v>63</v>
       </c>
       <c r="C64">
-        <v>233.2</v>
-      </c>
-      <c r="D64" s="32">
-        <v>200</v>
+        <f t="shared" si="0"/>
+        <v>214.79999999999976</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>185.20000000000013</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
@@ -6234,10 +6451,12 @@
         <v>64</v>
       </c>
       <c r="C65">
-        <v>236.4</v>
+        <f t="shared" si="0"/>
+        <v>217.99999999999974</v>
       </c>
       <c r="D65">
-        <v>202.8</v>
+        <f t="shared" si="1"/>
+        <v>188.00000000000014</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
@@ -6245,10 +6464,12 @@
         <v>65</v>
       </c>
       <c r="C66">
-        <v>239.6</v>
+        <f t="shared" si="0"/>
+        <v>221.19999999999973</v>
       </c>
       <c r="D66">
-        <v>205.6</v>
+        <f t="shared" si="1"/>
+        <v>190.80000000000015</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
@@ -6256,10 +6477,12 @@
         <v>66</v>
       </c>
       <c r="C67">
-        <v>242.8</v>
+        <f t="shared" si="0"/>
+        <v>224.39999999999972</v>
       </c>
       <c r="D67">
-        <v>208.4</v>
+        <f t="shared" si="1"/>
+        <v>193.60000000000016</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
@@ -6267,10 +6490,12 @@
         <v>67</v>
       </c>
       <c r="C68">
-        <v>246</v>
+        <f t="shared" ref="C68:C131" si="2">C67+3.2</f>
+        <v>227.59999999999971</v>
       </c>
       <c r="D68">
-        <v>211.2</v>
+        <f t="shared" ref="D68:D131" si="3">D67+2.8</f>
+        <v>196.40000000000018</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
@@ -6278,21 +6503,25 @@
         <v>68</v>
       </c>
       <c r="C69">
-        <v>249.2</v>
+        <f t="shared" si="2"/>
+        <v>230.7999999999997</v>
       </c>
       <c r="D69">
-        <v>214</v>
+        <f t="shared" si="3"/>
+        <v>199.20000000000019</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>69</v>
       </c>
-      <c r="C70" s="32">
-        <v>252.4</v>
+      <c r="C70">
+        <f t="shared" si="2"/>
+        <v>233.99999999999969</v>
       </c>
       <c r="D70">
-        <v>216.8</v>
+        <f t="shared" si="3"/>
+        <v>202.0000000000002</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
@@ -6300,10 +6529,12 @@
         <v>70</v>
       </c>
       <c r="C71">
-        <v>255.6</v>
+        <f t="shared" si="2"/>
+        <v>237.19999999999968</v>
       </c>
       <c r="D71">
-        <v>219.6</v>
+        <f t="shared" si="3"/>
+        <v>204.80000000000021</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
@@ -6311,10 +6542,12 @@
         <v>71</v>
       </c>
       <c r="C72">
-        <v>258.8</v>
+        <f t="shared" si="2"/>
+        <v>240.39999999999966</v>
       </c>
       <c r="D72">
-        <v>222.4</v>
+        <f t="shared" si="3"/>
+        <v>207.60000000000022</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
@@ -6322,10 +6555,12 @@
         <v>72</v>
       </c>
       <c r="C73">
-        <v>262</v>
-      </c>
-      <c r="D73" s="32">
-        <v>225.2</v>
+        <f t="shared" si="2"/>
+        <v>243.59999999999965</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="3"/>
+        <v>210.40000000000023</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
@@ -6333,10 +6568,12 @@
         <v>73</v>
       </c>
       <c r="C74">
-        <v>265.2</v>
+        <f t="shared" si="2"/>
+        <v>246.79999999999964</v>
       </c>
       <c r="D74">
-        <v>228</v>
+        <f t="shared" si="3"/>
+        <v>213.20000000000024</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
@@ -6344,10 +6581,12 @@
         <v>74</v>
       </c>
       <c r="C75">
-        <v>268.39999999999998</v>
+        <f t="shared" si="2"/>
+        <v>249.99999999999963</v>
       </c>
       <c r="D75">
-        <v>230.8</v>
+        <f t="shared" si="3"/>
+        <v>216.00000000000026</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
@@ -6355,21 +6594,25 @@
         <v>75</v>
       </c>
       <c r="C76">
-        <v>271.60000000000002</v>
+        <f t="shared" si="2"/>
+        <v>253.19999999999962</v>
       </c>
       <c r="D76">
-        <v>233.6</v>
+        <f t="shared" si="3"/>
+        <v>218.80000000000027</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>76</v>
       </c>
-      <c r="C77" s="32">
-        <v>274.8</v>
+      <c r="C77">
+        <f t="shared" si="2"/>
+        <v>256.39999999999964</v>
       </c>
       <c r="D77">
-        <v>236.4</v>
+        <f t="shared" si="3"/>
+        <v>221.60000000000028</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
@@ -6377,10 +6620,12 @@
         <v>77</v>
       </c>
       <c r="C78">
-        <v>278</v>
+        <f t="shared" si="2"/>
+        <v>259.59999999999962</v>
       </c>
       <c r="D78">
-        <v>239.2</v>
+        <f t="shared" si="3"/>
+        <v>224.40000000000029</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
@@ -6388,10 +6633,12 @@
         <v>78</v>
       </c>
       <c r="C79">
-        <v>281.2</v>
+        <f t="shared" si="2"/>
+        <v>262.79999999999961</v>
       </c>
       <c r="D79">
-        <v>242</v>
+        <f t="shared" si="3"/>
+        <v>227.2000000000003</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
@@ -6399,10 +6646,12 @@
         <v>79</v>
       </c>
       <c r="C80">
-        <v>284.39999999999998</v>
+        <f t="shared" si="2"/>
+        <v>265.9999999999996</v>
       </c>
       <c r="D80">
-        <v>244.8</v>
+        <f t="shared" si="3"/>
+        <v>230.00000000000031</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
@@ -6410,10 +6659,12 @@
         <v>80</v>
       </c>
       <c r="C81">
-        <v>287.60000000000002</v>
+        <f t="shared" si="2"/>
+        <v>269.19999999999959</v>
       </c>
       <c r="D81">
-        <v>247.6</v>
+        <f t="shared" si="3"/>
+        <v>232.80000000000032</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
@@ -6421,10 +6672,12 @@
         <v>81</v>
       </c>
       <c r="C82">
-        <v>290.8</v>
-      </c>
-      <c r="D82" s="32">
-        <v>250.4</v>
+        <f t="shared" si="2"/>
+        <v>272.39999999999958</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="3"/>
+        <v>235.60000000000034</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
@@ -6432,10 +6685,12 @@
         <v>82</v>
       </c>
       <c r="C83">
-        <v>294</v>
+        <f t="shared" si="2"/>
+        <v>275.59999999999957</v>
       </c>
       <c r="D83">
-        <v>253.2</v>
+        <f t="shared" si="3"/>
+        <v>238.40000000000035</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
@@ -6443,21 +6698,25 @@
         <v>83</v>
       </c>
       <c r="C84">
-        <v>297.2</v>
+        <f t="shared" si="2"/>
+        <v>278.79999999999956</v>
       </c>
       <c r="D84">
-        <v>256</v>
+        <f t="shared" si="3"/>
+        <v>241.20000000000036</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>84</v>
       </c>
-      <c r="C85" s="32">
-        <v>300.39999999999998</v>
+      <c r="C85">
+        <f t="shared" si="2"/>
+        <v>281.99999999999955</v>
       </c>
       <c r="D85">
-        <v>258.8</v>
+        <f t="shared" si="3"/>
+        <v>244.00000000000037</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
@@ -6465,10 +6724,12 @@
         <v>85</v>
       </c>
       <c r="C86">
-        <v>303.60000000000002</v>
+        <f t="shared" si="2"/>
+        <v>285.19999999999953</v>
       </c>
       <c r="D86">
-        <v>261.60000000000002</v>
+        <f t="shared" si="3"/>
+        <v>246.80000000000038</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
@@ -6476,10 +6737,12 @@
         <v>86</v>
       </c>
       <c r="C87">
-        <v>306.8</v>
+        <f t="shared" si="2"/>
+        <v>288.39999999999952</v>
       </c>
       <c r="D87">
-        <v>264.39999999999998</v>
+        <f t="shared" si="3"/>
+        <v>249.60000000000039</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
@@ -6487,10 +6750,12 @@
         <v>87</v>
       </c>
       <c r="C88">
-        <v>310</v>
+        <f t="shared" si="2"/>
+        <v>291.59999999999951</v>
       </c>
       <c r="D88">
-        <v>267.2</v>
+        <f t="shared" si="3"/>
+        <v>252.4000000000004</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
@@ -6498,10 +6763,12 @@
         <v>88</v>
       </c>
       <c r="C89">
-        <v>313.2</v>
+        <f t="shared" si="2"/>
+        <v>294.7999999999995</v>
       </c>
       <c r="D89">
-        <v>270</v>
+        <f t="shared" si="3"/>
+        <v>255.20000000000041</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
@@ -6509,10 +6776,12 @@
         <v>89</v>
       </c>
       <c r="C90">
-        <v>316.39999999999998</v>
+        <f t="shared" si="2"/>
+        <v>297.99999999999949</v>
       </c>
       <c r="D90">
-        <v>272.8</v>
+        <f t="shared" si="3"/>
+        <v>258.0000000000004</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
@@ -6520,10 +6789,12 @@
         <v>90</v>
       </c>
       <c r="C91">
-        <v>319.60000000000002</v>
-      </c>
-      <c r="D91" s="32">
-        <v>275.60000000000002</v>
+        <f t="shared" si="2"/>
+        <v>301.19999999999948</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="3"/>
+        <v>260.80000000000041</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
@@ -6531,21 +6802,25 @@
         <v>91</v>
       </c>
       <c r="C92">
-        <v>322.8</v>
+        <f t="shared" si="2"/>
+        <v>304.39999999999947</v>
       </c>
       <c r="D92">
-        <v>278.39999999999998</v>
+        <f t="shared" si="3"/>
+        <v>263.60000000000042</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>92</v>
       </c>
-      <c r="C93" s="32">
-        <v>326</v>
+      <c r="C93">
+        <f t="shared" si="2"/>
+        <v>307.59999999999945</v>
       </c>
       <c r="D93">
-        <v>281.2</v>
+        <f t="shared" si="3"/>
+        <v>266.40000000000043</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
@@ -6553,10 +6828,12 @@
         <v>93</v>
       </c>
       <c r="C94">
-        <v>329.2</v>
+        <f t="shared" si="2"/>
+        <v>310.79999999999944</v>
       </c>
       <c r="D94">
-        <v>284</v>
+        <f t="shared" si="3"/>
+        <v>269.20000000000044</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
@@ -6564,10 +6841,12 @@
         <v>94</v>
       </c>
       <c r="C95">
-        <v>332.4</v>
+        <f t="shared" si="2"/>
+        <v>313.99999999999943</v>
       </c>
       <c r="D95">
-        <v>286.8</v>
+        <f t="shared" si="3"/>
+        <v>272.00000000000045</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
@@ -6575,10 +6854,12 @@
         <v>95</v>
       </c>
       <c r="C96">
-        <v>335.6</v>
+        <f t="shared" si="2"/>
+        <v>317.19999999999942</v>
       </c>
       <c r="D96">
-        <v>289.60000000000002</v>
+        <f t="shared" si="3"/>
+        <v>274.80000000000047</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
@@ -6586,10 +6867,12 @@
         <v>96</v>
       </c>
       <c r="C97">
-        <v>338.8</v>
+        <f t="shared" si="2"/>
+        <v>320.39999999999941</v>
       </c>
       <c r="D97">
-        <v>292.39999999999998</v>
+        <f t="shared" si="3"/>
+        <v>277.60000000000048</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -6597,10 +6880,12 @@
         <v>97</v>
       </c>
       <c r="C98">
-        <v>342</v>
+        <f t="shared" si="2"/>
+        <v>323.5999999999994</v>
       </c>
       <c r="D98">
-        <v>295.2</v>
+        <f t="shared" si="3"/>
+        <v>280.40000000000049</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -6608,10 +6893,12 @@
         <v>98</v>
       </c>
       <c r="C99">
-        <v>345.2</v>
+        <f t="shared" si="2"/>
+        <v>326.79999999999939</v>
       </c>
       <c r="D99">
-        <v>298</v>
+        <f t="shared" si="3"/>
+        <v>283.2000000000005</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
@@ -6619,21 +6906,25 @@
         <v>99</v>
       </c>
       <c r="C100">
-        <v>348.4</v>
-      </c>
-      <c r="D100" s="32">
-        <v>300.8</v>
+        <f t="shared" si="2"/>
+        <v>329.99999999999937</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="3"/>
+        <v>286.00000000000051</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>100</v>
       </c>
-      <c r="C101" s="32">
-        <v>351.6</v>
+      <c r="C101">
+        <f t="shared" si="2"/>
+        <v>333.19999999999936</v>
       </c>
       <c r="D101">
-        <v>303.60000000000002</v>
+        <f t="shared" si="3"/>
+        <v>288.80000000000052</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
@@ -6641,10 +6932,12 @@
         <v>101</v>
       </c>
       <c r="C102">
-        <v>354.8</v>
+        <f t="shared" si="2"/>
+        <v>336.39999999999935</v>
       </c>
       <c r="D102">
-        <v>306.39999999999998</v>
+        <f t="shared" si="3"/>
+        <v>291.60000000000053</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
@@ -6652,10 +6945,12 @@
         <v>102</v>
       </c>
       <c r="C103">
-        <v>358</v>
+        <f t="shared" si="2"/>
+        <v>339.59999999999934</v>
       </c>
       <c r="D103">
-        <v>309.2</v>
+        <f t="shared" si="3"/>
+        <v>294.40000000000055</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
@@ -6663,10 +6958,12 @@
         <v>103</v>
       </c>
       <c r="C104">
-        <v>361.2</v>
+        <f t="shared" si="2"/>
+        <v>342.79999999999933</v>
       </c>
       <c r="D104">
-        <v>312</v>
+        <f t="shared" si="3"/>
+        <v>297.20000000000056</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
@@ -6674,10 +6971,12 @@
         <v>104</v>
       </c>
       <c r="C105">
-        <v>364.4</v>
+        <f t="shared" si="2"/>
+        <v>345.99999999999932</v>
       </c>
       <c r="D105">
-        <v>314.8</v>
+        <f t="shared" si="3"/>
+        <v>300.00000000000057</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
@@ -6685,10 +6984,12 @@
         <v>105</v>
       </c>
       <c r="C106">
-        <v>367.6</v>
+        <f t="shared" si="2"/>
+        <v>349.19999999999931</v>
       </c>
       <c r="D106">
-        <v>317.60000000000002</v>
+        <f t="shared" si="3"/>
+        <v>302.80000000000058</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
@@ -6696,10 +6997,12 @@
         <v>106</v>
       </c>
       <c r="C107">
-        <v>370.8</v>
+        <f t="shared" si="2"/>
+        <v>352.3999999999993</v>
       </c>
       <c r="D107">
-        <v>320.39999999999998</v>
+        <f t="shared" si="3"/>
+        <v>305.60000000000059</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
@@ -6707,21 +7010,25 @@
         <v>107</v>
       </c>
       <c r="C108">
-        <v>374</v>
+        <f t="shared" si="2"/>
+        <v>355.59999999999928</v>
       </c>
       <c r="D108">
-        <v>323.2</v>
+        <f t="shared" si="3"/>
+        <v>308.4000000000006</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>108</v>
       </c>
-      <c r="C109" s="32">
-        <v>377.2</v>
-      </c>
-      <c r="D109" s="32">
-        <v>326</v>
+      <c r="C109">
+        <f t="shared" si="2"/>
+        <v>358.79999999999927</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="3"/>
+        <v>311.20000000000061</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
@@ -6729,10 +7036,12 @@
         <v>109</v>
       </c>
       <c r="C110">
-        <v>380.4</v>
+        <f t="shared" si="2"/>
+        <v>361.99999999999926</v>
       </c>
       <c r="D110">
-        <v>328.8</v>
+        <f t="shared" si="3"/>
+        <v>314.00000000000063</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
@@ -6740,10 +7049,12 @@
         <v>110</v>
       </c>
       <c r="C111">
-        <v>383.6</v>
+        <f t="shared" si="2"/>
+        <v>365.19999999999925</v>
       </c>
       <c r="D111">
-        <v>331.6</v>
+        <f t="shared" si="3"/>
+        <v>316.80000000000064</v>
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
@@ -6751,10 +7062,12 @@
         <v>111</v>
       </c>
       <c r="C112">
-        <v>386.8</v>
+        <f t="shared" si="2"/>
+        <v>368.39999999999924</v>
       </c>
       <c r="D112">
-        <v>334.4</v>
+        <f t="shared" si="3"/>
+        <v>319.60000000000065</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
@@ -6762,10 +7075,12 @@
         <v>112</v>
       </c>
       <c r="C113">
-        <v>390</v>
+        <f t="shared" si="2"/>
+        <v>371.59999999999923</v>
       </c>
       <c r="D113">
-        <v>337.2</v>
+        <f t="shared" si="3"/>
+        <v>322.40000000000066</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
@@ -6773,10 +7088,12 @@
         <v>113</v>
       </c>
       <c r="C114">
-        <v>393.2</v>
+        <f t="shared" si="2"/>
+        <v>374.79999999999922</v>
       </c>
       <c r="D114">
-        <v>340</v>
+        <f t="shared" si="3"/>
+        <v>325.20000000000067</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
@@ -6784,21 +7101,25 @@
         <v>114</v>
       </c>
       <c r="C115">
-        <v>396.4</v>
+        <f t="shared" si="2"/>
+        <v>377.9999999999992</v>
       </c>
       <c r="D115">
-        <v>342.8</v>
+        <f t="shared" si="3"/>
+        <v>328.00000000000068</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>115</v>
       </c>
-      <c r="C116" s="32">
-        <v>399.6</v>
+      <c r="C116">
+        <f t="shared" si="2"/>
+        <v>381.19999999999919</v>
       </c>
       <c r="D116">
-        <v>345.6</v>
+        <f t="shared" si="3"/>
+        <v>330.80000000000069</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
@@ -6806,10 +7127,12 @@
         <v>116</v>
       </c>
       <c r="C117">
-        <v>402.8</v>
+        <f t="shared" si="2"/>
+        <v>384.39999999999918</v>
       </c>
       <c r="D117">
-        <v>348.4</v>
+        <f t="shared" si="3"/>
+        <v>333.6000000000007</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
@@ -6817,10 +7140,12 @@
         <v>117</v>
       </c>
       <c r="C118">
-        <v>406</v>
-      </c>
-      <c r="D118" s="32">
-        <v>351.2</v>
+        <f t="shared" si="2"/>
+        <v>387.59999999999917</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="3"/>
+        <v>336.40000000000072</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
@@ -6828,10 +7153,12 @@
         <v>118</v>
       </c>
       <c r="C119">
-        <v>409.2</v>
+        <f t="shared" si="2"/>
+        <v>390.79999999999916</v>
       </c>
       <c r="D119">
-        <v>354</v>
+        <f t="shared" si="3"/>
+        <v>339.20000000000073</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
@@ -6839,10 +7166,12 @@
         <v>119</v>
       </c>
       <c r="C120">
-        <v>412.4</v>
+        <f t="shared" si="2"/>
+        <v>393.99999999999915</v>
       </c>
       <c r="D120">
-        <v>356.8</v>
+        <f t="shared" si="3"/>
+        <v>342.00000000000074</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
@@ -6850,10 +7179,12 @@
         <v>120</v>
       </c>
       <c r="C121">
-        <v>415.6</v>
+        <f t="shared" si="2"/>
+        <v>397.19999999999914</v>
       </c>
       <c r="D121">
-        <v>359.6</v>
+        <f t="shared" si="3"/>
+        <v>344.80000000000075</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
@@ -6861,10 +7192,12 @@
         <v>121</v>
       </c>
       <c r="C122">
-        <v>418.8</v>
+        <f t="shared" si="2"/>
+        <v>400.39999999999912</v>
       </c>
       <c r="D122">
-        <v>362.4</v>
+        <f t="shared" si="3"/>
+        <v>347.60000000000076</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
@@ -6872,21 +7205,25 @@
         <v>122</v>
       </c>
       <c r="C123">
-        <v>422</v>
+        <f t="shared" si="2"/>
+        <v>403.59999999999911</v>
       </c>
       <c r="D123">
-        <v>365.2</v>
+        <f t="shared" si="3"/>
+        <v>350.40000000000077</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>123</v>
       </c>
-      <c r="C124" s="32">
-        <v>425.2</v>
+      <c r="C124">
+        <f t="shared" si="2"/>
+        <v>406.7999999999991</v>
       </c>
       <c r="D124">
-        <v>368</v>
+        <f t="shared" si="3"/>
+        <v>353.20000000000078</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
@@ -6894,10 +7231,12 @@
         <v>124</v>
       </c>
       <c r="C125">
-        <v>428.4</v>
+        <f t="shared" si="2"/>
+        <v>409.99999999999909</v>
       </c>
       <c r="D125">
-        <v>370.8</v>
+        <f t="shared" si="3"/>
+        <v>356.0000000000008</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
@@ -6905,10 +7244,12 @@
         <v>125</v>
       </c>
       <c r="C126">
-        <v>431.6</v>
+        <f t="shared" si="2"/>
+        <v>413.19999999999908</v>
       </c>
       <c r="D126">
-        <v>373.6</v>
+        <f t="shared" si="3"/>
+        <v>358.80000000000081</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
@@ -6916,10 +7257,12 @@
         <v>126</v>
       </c>
       <c r="C127">
-        <v>434.8</v>
-      </c>
-      <c r="D127" s="32">
-        <v>376.4</v>
+        <f t="shared" si="2"/>
+        <v>416.39999999999907</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="3"/>
+        <v>361.60000000000082</v>
       </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
@@ -6927,10 +7270,12 @@
         <v>127</v>
       </c>
       <c r="C128">
-        <v>438</v>
+        <f t="shared" si="2"/>
+        <v>419.59999999999906</v>
       </c>
       <c r="D128">
-        <v>379.2</v>
+        <f t="shared" si="3"/>
+        <v>364.40000000000083</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
@@ -6938,10 +7283,12 @@
         <v>128</v>
       </c>
       <c r="C129">
-        <v>441.2</v>
+        <f t="shared" si="2"/>
+        <v>422.79999999999905</v>
       </c>
       <c r="D129">
-        <v>382</v>
+        <f t="shared" si="3"/>
+        <v>367.20000000000084</v>
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
@@ -6949,10 +7296,12 @@
         <v>129</v>
       </c>
       <c r="C130">
-        <v>444.4</v>
+        <f t="shared" si="2"/>
+        <v>425.99999999999903</v>
       </c>
       <c r="D130">
-        <v>384.8</v>
+        <f t="shared" si="3"/>
+        <v>370.00000000000085</v>
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
@@ -6960,21 +7309,25 @@
         <v>130</v>
       </c>
       <c r="C131">
-        <v>447.6</v>
+        <f t="shared" si="2"/>
+        <v>429.19999999999902</v>
       </c>
       <c r="D131">
-        <v>387.6</v>
+        <f t="shared" si="3"/>
+        <v>372.80000000000086</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132">
         <v>131</v>
       </c>
-      <c r="C132" s="32">
-        <v>450.8</v>
+      <c r="C132">
+        <f t="shared" ref="C132:C195" si="4">C131+3.2</f>
+        <v>432.39999999999901</v>
       </c>
       <c r="D132">
-        <v>390.4</v>
+        <f t="shared" ref="D132:D195" si="5">D131+2.8</f>
+        <v>375.60000000000088</v>
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
@@ -6982,10 +7335,12 @@
         <v>132</v>
       </c>
       <c r="C133">
-        <v>454</v>
+        <f t="shared" si="4"/>
+        <v>435.599999999999</v>
       </c>
       <c r="D133">
-        <v>393.2</v>
+        <f t="shared" si="5"/>
+        <v>378.40000000000089</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
@@ -6993,10 +7348,12 @@
         <v>133</v>
       </c>
       <c r="C134">
-        <v>457.2</v>
+        <f t="shared" si="4"/>
+        <v>438.79999999999899</v>
       </c>
       <c r="D134">
-        <v>396</v>
+        <f t="shared" si="5"/>
+        <v>381.2000000000009</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
@@ -7004,10 +7361,12 @@
         <v>134</v>
       </c>
       <c r="C135">
-        <v>460.4</v>
-      </c>
-      <c r="D135" s="32">
-        <v>398.8</v>
+        <f t="shared" si="4"/>
+        <v>441.99999999999898</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="5"/>
+        <v>384.00000000000091</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
@@ -7015,10 +7374,12 @@
         <v>135</v>
       </c>
       <c r="C136">
-        <v>463.6</v>
+        <f t="shared" si="4"/>
+        <v>445.19999999999897</v>
       </c>
       <c r="D136">
-        <v>401.6</v>
+        <f t="shared" si="5"/>
+        <v>386.80000000000092</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
@@ -7026,10 +7387,12 @@
         <v>136</v>
       </c>
       <c r="C137">
-        <v>466.8</v>
+        <f t="shared" si="4"/>
+        <v>448.39999999999895</v>
       </c>
       <c r="D137">
-        <v>404.4</v>
+        <f t="shared" si="5"/>
+        <v>389.60000000000093</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
@@ -7037,10 +7400,12 @@
         <v>137</v>
       </c>
       <c r="C138">
-        <v>470</v>
+        <f t="shared" si="4"/>
+        <v>451.59999999999894</v>
       </c>
       <c r="D138">
-        <v>407.2</v>
+        <f t="shared" si="5"/>
+        <v>392.40000000000094</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
@@ -7048,21 +7413,25 @@
         <v>138</v>
       </c>
       <c r="C139">
-        <v>473.2</v>
+        <f t="shared" si="4"/>
+        <v>454.79999999999893</v>
       </c>
       <c r="D139">
-        <v>410</v>
+        <f t="shared" si="5"/>
+        <v>395.20000000000095</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140">
         <v>139</v>
       </c>
-      <c r="C140" s="32">
-        <v>476.4</v>
+      <c r="C140">
+        <f t="shared" si="4"/>
+        <v>457.99999999999892</v>
       </c>
       <c r="D140">
-        <v>412.8</v>
+        <f t="shared" si="5"/>
+        <v>398.00000000000097</v>
       </c>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
@@ -7070,10 +7439,12 @@
         <v>140</v>
       </c>
       <c r="C141">
-        <v>479.6</v>
+        <f t="shared" si="4"/>
+        <v>461.19999999999891</v>
       </c>
       <c r="D141">
-        <v>415.6</v>
+        <f t="shared" si="5"/>
+        <v>400.80000000000098</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
@@ -7081,10 +7452,12 @@
         <v>141</v>
       </c>
       <c r="C142">
-        <v>482.8</v>
+        <f t="shared" si="4"/>
+        <v>464.3999999999989</v>
       </c>
       <c r="D142">
-        <v>418.4</v>
+        <f t="shared" si="5"/>
+        <v>403.60000000000099</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
@@ -7092,10 +7465,12 @@
         <v>142</v>
       </c>
       <c r="C143">
-        <v>486</v>
+        <f t="shared" si="4"/>
+        <v>467.59999999999889</v>
       </c>
       <c r="D143">
-        <v>421.2</v>
+        <f t="shared" si="5"/>
+        <v>406.400000000001</v>
       </c>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
@@ -7103,10 +7478,12 @@
         <v>143</v>
       </c>
       <c r="C144">
-        <v>489.2</v>
+        <f t="shared" si="4"/>
+        <v>470.79999999999887</v>
       </c>
       <c r="D144">
-        <v>424</v>
+        <f t="shared" si="5"/>
+        <v>409.20000000000101</v>
       </c>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
@@ -7114,10 +7491,12 @@
         <v>144</v>
       </c>
       <c r="C145">
-        <v>492.4</v>
-      </c>
-      <c r="D145" s="32">
-        <v>426.8</v>
+        <f t="shared" si="4"/>
+        <v>473.99999999999886</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="5"/>
+        <v>412.00000000000102</v>
       </c>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
@@ -7125,21 +7504,25 @@
         <v>145</v>
       </c>
       <c r="C146">
-        <v>495.6</v>
+        <f t="shared" si="4"/>
+        <v>477.19999999999885</v>
       </c>
       <c r="D146">
-        <v>429.6</v>
+        <f t="shared" si="5"/>
+        <v>414.80000000000103</v>
       </c>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147">
         <v>146</v>
       </c>
-      <c r="C147" s="32">
-        <v>498.8</v>
+      <c r="C147">
+        <f t="shared" si="4"/>
+        <v>480.39999999999884</v>
       </c>
       <c r="D147">
-        <v>432.4</v>
+        <f t="shared" si="5"/>
+        <v>417.60000000000105</v>
       </c>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
@@ -7147,10 +7530,12 @@
         <v>147</v>
       </c>
       <c r="C148">
-        <v>502</v>
+        <f t="shared" si="4"/>
+        <v>483.59999999999883</v>
       </c>
       <c r="D148">
-        <v>435.2</v>
+        <f t="shared" si="5"/>
+        <v>420.40000000000106</v>
       </c>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
@@ -7158,10 +7543,12 @@
         <v>148</v>
       </c>
       <c r="C149">
-        <v>505.2</v>
+        <f t="shared" si="4"/>
+        <v>486.79999999999882</v>
       </c>
       <c r="D149">
-        <v>438</v>
+        <f t="shared" si="5"/>
+        <v>423.20000000000107</v>
       </c>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
@@ -7169,10 +7556,12 @@
         <v>149</v>
       </c>
       <c r="C150">
-        <v>508.4</v>
+        <f t="shared" si="4"/>
+        <v>489.99999999999881</v>
       </c>
       <c r="D150">
-        <v>440.8</v>
+        <f t="shared" si="5"/>
+        <v>426.00000000000108</v>
       </c>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
@@ -7180,10 +7569,12 @@
         <v>150</v>
       </c>
       <c r="C151">
-        <v>511.6</v>
+        <f t="shared" si="4"/>
+        <v>493.19999999999879</v>
       </c>
       <c r="D151">
-        <v>443.6</v>
+        <f t="shared" si="5"/>
+        <v>428.80000000000109</v>
       </c>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
@@ -7191,10 +7582,12 @@
         <v>151</v>
       </c>
       <c r="C152">
-        <v>514.79999999999995</v>
+        <f t="shared" si="4"/>
+        <v>496.39999999999878</v>
       </c>
       <c r="D152">
-        <v>446.4</v>
+        <f t="shared" si="5"/>
+        <v>431.6000000000011</v>
       </c>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
@@ -7202,10 +7595,12 @@
         <v>152</v>
       </c>
       <c r="C153">
-        <v>518</v>
-      </c>
-      <c r="D153" s="32">
-        <v>449.2</v>
+        <f t="shared" si="4"/>
+        <v>499.59999999999877</v>
+      </c>
+      <c r="D153">
+        <f t="shared" si="5"/>
+        <v>434.40000000000111</v>
       </c>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
@@ -7213,10 +7608,12 @@
         <v>153</v>
       </c>
       <c r="C154">
-        <v>521.20000000000005</v>
+        <f t="shared" si="4"/>
+        <v>502.79999999999876</v>
       </c>
       <c r="D154">
-        <v>452</v>
+        <f t="shared" si="5"/>
+        <v>437.20000000000113</v>
       </c>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
@@ -7224,10 +7621,12 @@
         <v>154</v>
       </c>
       <c r="C155">
-        <v>524.4</v>
+        <f t="shared" si="4"/>
+        <v>505.99999999999875</v>
       </c>
       <c r="D155">
-        <v>454.8</v>
+        <f t="shared" si="5"/>
+        <v>440.00000000000114</v>
       </c>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
@@ -7235,10 +7634,12 @@
         <v>155</v>
       </c>
       <c r="C156">
-        <v>527.6</v>
+        <f t="shared" si="4"/>
+        <v>509.19999999999874</v>
       </c>
       <c r="D156">
-        <v>457.6</v>
+        <f t="shared" si="5"/>
+        <v>442.80000000000115</v>
       </c>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
@@ -7246,10 +7647,12 @@
         <v>156</v>
       </c>
       <c r="C157">
-        <v>530.79999999999995</v>
+        <f t="shared" si="4"/>
+        <v>512.39999999999873</v>
       </c>
       <c r="D157">
-        <v>460.4</v>
+        <f t="shared" si="5"/>
+        <v>445.60000000000116</v>
       </c>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
@@ -7257,10 +7660,12 @@
         <v>157</v>
       </c>
       <c r="C158">
-        <v>534</v>
+        <f t="shared" si="4"/>
+        <v>515.59999999999877</v>
       </c>
       <c r="D158">
-        <v>463.2</v>
+        <f t="shared" si="5"/>
+        <v>448.40000000000117</v>
       </c>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
@@ -7268,10 +7673,12 @@
         <v>158</v>
       </c>
       <c r="C159">
-        <v>537.20000000000005</v>
+        <f t="shared" si="4"/>
+        <v>518.79999999999882</v>
       </c>
       <c r="D159">
-        <v>466</v>
+        <f t="shared" si="5"/>
+        <v>451.20000000000118</v>
       </c>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
@@ -7279,10 +7686,12 @@
         <v>159</v>
       </c>
       <c r="C160">
-        <v>540.4</v>
+        <f t="shared" si="4"/>
+        <v>521.99999999999886</v>
       </c>
       <c r="D160">
-        <v>468.8</v>
+        <f t="shared" si="5"/>
+        <v>454.00000000000119</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
@@ -7290,10 +7699,12 @@
         <v>160</v>
       </c>
       <c r="C161">
-        <v>543.6</v>
+        <f t="shared" si="4"/>
+        <v>525.19999999999891</v>
       </c>
       <c r="D161">
-        <v>471.6</v>
+        <f t="shared" si="5"/>
+        <v>456.80000000000121</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
@@ -7301,10 +7712,12 @@
         <v>161</v>
       </c>
       <c r="C162">
-        <v>546.79999999999995</v>
+        <f t="shared" si="4"/>
+        <v>528.39999999999895</v>
       </c>
       <c r="D162">
-        <v>474.4</v>
+        <f t="shared" si="5"/>
+        <v>459.60000000000122</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
@@ -7312,10 +7725,12 @@
         <v>162</v>
       </c>
       <c r="C163">
-        <v>550.00000000000102</v>
-      </c>
-      <c r="D163" s="32">
-        <v>477.2</v>
+        <f t="shared" si="4"/>
+        <v>531.599999999999</v>
+      </c>
+      <c r="D163">
+        <f t="shared" si="5"/>
+        <v>462.40000000000123</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
@@ -7323,10 +7738,12 @@
         <v>163</v>
       </c>
       <c r="C164">
-        <v>553.20000000000005</v>
+        <f t="shared" si="4"/>
+        <v>534.79999999999905</v>
       </c>
       <c r="D164">
-        <v>480</v>
+        <f t="shared" si="5"/>
+        <v>465.20000000000124</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
@@ -7334,10 +7751,12 @@
         <v>164</v>
       </c>
       <c r="C165">
-        <v>556.4</v>
+        <f t="shared" si="4"/>
+        <v>537.99999999999909</v>
       </c>
       <c r="D165">
-        <v>482.8</v>
+        <f t="shared" si="5"/>
+        <v>468.00000000000125</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
@@ -7345,10 +7764,12 @@
         <v>165</v>
       </c>
       <c r="C166">
-        <v>559.6</v>
+        <f t="shared" si="4"/>
+        <v>541.19999999999914</v>
       </c>
       <c r="D166">
-        <v>485.6</v>
+        <f t="shared" si="5"/>
+        <v>470.80000000000126</v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
@@ -7356,10 +7777,12 @@
         <v>166</v>
       </c>
       <c r="C167">
-        <v>562.79999999999995</v>
+        <f t="shared" si="4"/>
+        <v>544.39999999999918</v>
       </c>
       <c r="D167">
-        <v>488.4</v>
+        <f t="shared" si="5"/>
+        <v>473.60000000000127</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
@@ -7367,10 +7790,12 @@
         <v>167</v>
       </c>
       <c r="C168">
-        <v>566.00000000000102</v>
+        <f t="shared" si="4"/>
+        <v>547.59999999999923</v>
       </c>
       <c r="D168">
-        <v>491.2</v>
+        <f t="shared" si="5"/>
+        <v>476.40000000000128</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
@@ -7378,10 +7803,12 @@
         <v>168</v>
       </c>
       <c r="C169">
-        <v>569.20000000000005</v>
+        <f t="shared" si="4"/>
+        <v>550.79999999999927</v>
       </c>
       <c r="D169">
-        <v>494</v>
+        <f t="shared" si="5"/>
+        <v>479.2000000000013</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
@@ -7389,10 +7816,12 @@
         <v>169</v>
       </c>
       <c r="C170">
-        <v>572.4</v>
+        <f t="shared" si="4"/>
+        <v>553.99999999999932</v>
       </c>
       <c r="D170">
-        <v>496.8</v>
+        <f t="shared" si="5"/>
+        <v>482.00000000000131</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
@@ -7400,10 +7829,12 @@
         <v>170</v>
       </c>
       <c r="C171">
-        <v>575.60000000000105</v>
-      </c>
-      <c r="D171" s="32">
-        <v>499.6</v>
+        <f t="shared" si="4"/>
+        <v>557.19999999999936</v>
+      </c>
+      <c r="D171">
+        <f t="shared" si="5"/>
+        <v>484.80000000000132</v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
@@ -7411,10 +7842,12 @@
         <v>171</v>
       </c>
       <c r="C172">
-        <v>578.79999999999995</v>
+        <f t="shared" si="4"/>
+        <v>560.39999999999941</v>
       </c>
       <c r="D172">
-        <v>502.4</v>
+        <f t="shared" si="5"/>
+        <v>487.60000000000133</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
@@ -7422,10 +7855,12 @@
         <v>172</v>
       </c>
       <c r="C173">
-        <v>582.00000000000102</v>
+        <f t="shared" si="4"/>
+        <v>563.59999999999945</v>
       </c>
       <c r="D173">
-        <v>505.2</v>
+        <f t="shared" si="5"/>
+        <v>490.40000000000134</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
@@ -7433,10 +7868,12 @@
         <v>173</v>
       </c>
       <c r="C174">
-        <v>585.20000000000095</v>
+        <f t="shared" si="4"/>
+        <v>566.7999999999995</v>
       </c>
       <c r="D174">
-        <v>508</v>
+        <f t="shared" si="5"/>
+        <v>493.20000000000135</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
@@ -7444,10 +7881,12 @@
         <v>174</v>
       </c>
       <c r="C175">
-        <v>588.4</v>
+        <f t="shared" si="4"/>
+        <v>569.99999999999955</v>
       </c>
       <c r="D175">
-        <v>510.8</v>
+        <f t="shared" si="5"/>
+        <v>496.00000000000136</v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
@@ -7455,10 +7894,12 @@
         <v>175</v>
       </c>
       <c r="C176">
-        <v>591.60000000000105</v>
+        <f t="shared" si="4"/>
+        <v>573.19999999999959</v>
       </c>
       <c r="D176">
-        <v>513.6</v>
+        <f t="shared" si="5"/>
+        <v>498.80000000000138</v>
       </c>
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.25">
@@ -7466,10 +7907,12 @@
         <v>176</v>
       </c>
       <c r="C177">
-        <v>594.79999999999995</v>
+        <f t="shared" si="4"/>
+        <v>576.39999999999964</v>
       </c>
       <c r="D177">
-        <v>516.4</v>
+        <f t="shared" si="5"/>
+        <v>501.60000000000139</v>
       </c>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.25">
@@ -7477,10 +7920,12 @@
         <v>177</v>
       </c>
       <c r="C178">
-        <v>598.00000000000102</v>
+        <f t="shared" si="4"/>
+        <v>579.59999999999968</v>
       </c>
       <c r="D178">
-        <v>519.20000000000005</v>
+        <f t="shared" si="5"/>
+        <v>504.4000000000014</v>
       </c>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.25">
@@ -7488,10 +7933,12 @@
         <v>178</v>
       </c>
       <c r="C179">
-        <v>601.20000000000095</v>
+        <f t="shared" si="4"/>
+        <v>582.79999999999973</v>
       </c>
       <c r="D179">
-        <v>522</v>
+        <f t="shared" si="5"/>
+        <v>507.20000000000141</v>
       </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
@@ -7499,10 +7946,12 @@
         <v>179</v>
       </c>
       <c r="C180">
-        <v>604.4</v>
+        <f t="shared" si="4"/>
+        <v>585.99999999999977</v>
       </c>
       <c r="D180">
-        <v>524.79999999999995</v>
+        <f t="shared" si="5"/>
+        <v>510.00000000000142</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.25">
@@ -7510,10 +7959,12 @@
         <v>180</v>
       </c>
       <c r="C181">
-        <v>607.60000000000105</v>
+        <f t="shared" si="4"/>
+        <v>589.19999999999982</v>
       </c>
       <c r="D181">
-        <v>527.6</v>
+        <f t="shared" si="5"/>
+        <v>512.80000000000143</v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.25">
@@ -7521,10 +7972,12 @@
         <v>181</v>
       </c>
       <c r="C182">
-        <v>610.79999999999995</v>
+        <f t="shared" si="4"/>
+        <v>592.39999999999986</v>
       </c>
       <c r="D182">
-        <v>530.4</v>
+        <f t="shared" si="5"/>
+        <v>515.60000000000139</v>
       </c>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.25">
@@ -7532,10 +7985,12 @@
         <v>182</v>
       </c>
       <c r="C183">
-        <v>614.00000000000102</v>
+        <f t="shared" si="4"/>
+        <v>595.59999999999991</v>
       </c>
       <c r="D183">
-        <v>533.20000000000005</v>
+        <f t="shared" si="5"/>
+        <v>518.40000000000134</v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
@@ -7543,10 +7998,12 @@
         <v>183</v>
       </c>
       <c r="C184">
-        <v>617.20000000000095</v>
+        <f t="shared" si="4"/>
+        <v>598.79999999999995</v>
       </c>
       <c r="D184">
-        <v>536</v>
+        <f t="shared" si="5"/>
+        <v>521.2000000000013</v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
@@ -7554,10 +8011,12 @@
         <v>184</v>
       </c>
       <c r="C185">
-        <v>620.4</v>
+        <f t="shared" si="4"/>
+        <v>602</v>
       </c>
       <c r="D185">
-        <v>538.79999999999995</v>
+        <f t="shared" si="5"/>
+        <v>524.00000000000125</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.25">
@@ -7565,10 +8024,12 @@
         <v>185</v>
       </c>
       <c r="C186">
-        <v>623.60000000000105</v>
+        <f t="shared" si="4"/>
+        <v>605.20000000000005</v>
       </c>
       <c r="D186">
-        <v>541.6</v>
+        <f t="shared" si="5"/>
+        <v>526.80000000000121</v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.25">
@@ -7576,10 +8037,12 @@
         <v>186</v>
       </c>
       <c r="C187">
-        <v>626.80000000000098</v>
+        <f t="shared" si="4"/>
+        <v>608.40000000000009</v>
       </c>
       <c r="D187">
-        <v>544.4</v>
+        <f t="shared" si="5"/>
+        <v>529.60000000000116</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
@@ -7587,10 +8050,12 @@
         <v>187</v>
       </c>
       <c r="C188">
-        <v>630.00000000000102</v>
+        <f t="shared" si="4"/>
+        <v>611.60000000000014</v>
       </c>
       <c r="D188">
-        <v>547.20000000000005</v>
+        <f t="shared" si="5"/>
+        <v>532.40000000000111</v>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
@@ -7598,10 +8063,12 @@
         <v>188</v>
       </c>
       <c r="C189">
-        <v>633.20000000000095</v>
+        <f t="shared" si="4"/>
+        <v>614.80000000000018</v>
       </c>
       <c r="D189">
-        <v>550</v>
+        <f t="shared" si="5"/>
+        <v>535.20000000000107</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
@@ -7609,10 +8076,12 @@
         <v>189</v>
       </c>
       <c r="C190">
-        <v>636.400000000001</v>
+        <f t="shared" si="4"/>
+        <v>618.00000000000023</v>
       </c>
       <c r="D190">
-        <v>552.79999999999995</v>
+        <f t="shared" si="5"/>
+        <v>538.00000000000102</v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.25">
@@ -7620,10 +8089,12 @@
         <v>190</v>
       </c>
       <c r="C191">
-        <v>639.60000000000105</v>
+        <f t="shared" si="4"/>
+        <v>621.20000000000027</v>
       </c>
       <c r="D191">
-        <v>555.6</v>
+        <f t="shared" si="5"/>
+        <v>540.80000000000098</v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.25">
@@ -7631,10 +8102,12 @@
         <v>191</v>
       </c>
       <c r="C192">
-        <v>642.80000000000098</v>
+        <f t="shared" si="4"/>
+        <v>624.40000000000032</v>
       </c>
       <c r="D192">
-        <v>558.4</v>
+        <f t="shared" si="5"/>
+        <v>543.60000000000093</v>
       </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
@@ -7642,10 +8115,12 @@
         <v>192</v>
       </c>
       <c r="C193">
-        <v>646.00000000000102</v>
+        <f t="shared" si="4"/>
+        <v>627.60000000000036</v>
       </c>
       <c r="D193">
-        <v>561.20000000000005</v>
+        <f t="shared" si="5"/>
+        <v>546.40000000000089</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
@@ -7653,10 +8128,12 @@
         <v>193</v>
       </c>
       <c r="C194">
-        <v>649.20000000000095</v>
+        <f t="shared" si="4"/>
+        <v>630.80000000000041</v>
       </c>
       <c r="D194">
-        <v>564</v>
+        <f t="shared" si="5"/>
+        <v>549.20000000000084</v>
       </c>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
@@ -7664,10 +8141,12 @@
         <v>194</v>
       </c>
       <c r="C195">
-        <v>652.400000000001</v>
+        <f t="shared" si="4"/>
+        <v>634.00000000000045</v>
       </c>
       <c r="D195">
-        <v>566.79999999999995</v>
+        <f t="shared" si="5"/>
+        <v>552.0000000000008</v>
       </c>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
@@ -7675,10 +8154,12 @@
         <v>195</v>
       </c>
       <c r="C196">
-        <v>655.60000000000105</v>
+        <f t="shared" ref="C196:C257" si="6">C195+3.2</f>
+        <v>637.2000000000005</v>
       </c>
       <c r="D196">
-        <v>569.6</v>
+        <f t="shared" ref="D196:D257" si="7">D195+2.8</f>
+        <v>554.80000000000075</v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
@@ -7686,10 +8167,12 @@
         <v>196</v>
       </c>
       <c r="C197">
-        <v>658.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>640.40000000000055</v>
       </c>
       <c r="D197">
-        <v>572.4</v>
+        <f t="shared" si="7"/>
+        <v>557.6000000000007</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
@@ -7697,10 +8180,12 @@
         <v>197</v>
       </c>
       <c r="C198">
-        <v>662.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>643.60000000000059</v>
       </c>
       <c r="D198">
-        <v>575.20000000000005</v>
+        <f t="shared" si="7"/>
+        <v>560.40000000000066</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
@@ -7708,10 +8193,12 @@
         <v>198</v>
       </c>
       <c r="C199">
-        <v>665.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>646.80000000000064</v>
       </c>
       <c r="D199">
-        <v>578</v>
+        <f t="shared" si="7"/>
+        <v>563.20000000000061</v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
@@ -7719,10 +8206,12 @@
         <v>199</v>
       </c>
       <c r="C200">
-        <v>668.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>650.00000000000068</v>
       </c>
       <c r="D200">
-        <v>580.79999999999995</v>
+        <f t="shared" si="7"/>
+        <v>566.00000000000057</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
@@ -7730,10 +8219,12 @@
         <v>200</v>
       </c>
       <c r="C201">
-        <v>671.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>653.20000000000073</v>
       </c>
       <c r="D201">
-        <v>583.6</v>
+        <f t="shared" si="7"/>
+        <v>568.80000000000052</v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
@@ -7741,10 +8232,12 @@
         <v>201</v>
       </c>
       <c r="C202">
-        <v>674.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>656.40000000000077</v>
       </c>
       <c r="D202">
-        <v>586.4</v>
+        <f t="shared" si="7"/>
+        <v>571.60000000000048</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
@@ -7752,10 +8245,12 @@
         <v>202</v>
       </c>
       <c r="C203">
-        <v>678.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>659.60000000000082</v>
       </c>
       <c r="D203">
-        <v>589.20000000000005</v>
+        <f t="shared" si="7"/>
+        <v>574.40000000000043</v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
@@ -7763,10 +8258,12 @@
         <v>203</v>
       </c>
       <c r="C204">
-        <v>681.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>662.80000000000086</v>
       </c>
       <c r="D204">
-        <v>592</v>
+        <f t="shared" si="7"/>
+        <v>577.20000000000039</v>
       </c>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
@@ -7774,10 +8271,12 @@
         <v>204</v>
       </c>
       <c r="C205">
-        <v>684.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>666.00000000000091</v>
       </c>
       <c r="D205">
-        <v>594.79999999999995</v>
+        <f t="shared" si="7"/>
+        <v>580.00000000000034</v>
       </c>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
@@ -7785,10 +8284,12 @@
         <v>205</v>
       </c>
       <c r="C206">
-        <v>687.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>669.20000000000095</v>
       </c>
       <c r="D206">
-        <v>597.6</v>
+        <f t="shared" si="7"/>
+        <v>582.8000000000003</v>
       </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
@@ -7796,10 +8297,12 @@
         <v>206</v>
       </c>
       <c r="C207">
-        <v>690.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>672.400000000001</v>
       </c>
       <c r="D207">
-        <v>600.4</v>
+        <f t="shared" si="7"/>
+        <v>585.60000000000025</v>
       </c>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
@@ -7807,10 +8310,12 @@
         <v>207</v>
       </c>
       <c r="C208">
-        <v>694.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>675.60000000000105</v>
       </c>
       <c r="D208">
-        <v>603.20000000000005</v>
+        <f t="shared" si="7"/>
+        <v>588.4000000000002</v>
       </c>
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.25">
@@ -7818,10 +8323,12 @@
         <v>208</v>
       </c>
       <c r="C209">
-        <v>697.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>678.80000000000109</v>
       </c>
       <c r="D209">
-        <v>606</v>
+        <f t="shared" si="7"/>
+        <v>591.20000000000016</v>
       </c>
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.25">
@@ -7829,10 +8336,12 @@
         <v>209</v>
       </c>
       <c r="C210">
-        <v>700.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>682.00000000000114</v>
       </c>
       <c r="D210">
-        <v>608.79999999999995</v>
+        <f t="shared" si="7"/>
+        <v>594.00000000000011</v>
       </c>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.25">
@@ -7840,10 +8349,12 @@
         <v>210</v>
       </c>
       <c r="C211">
-        <v>703.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>685.20000000000118</v>
       </c>
       <c r="D211">
-        <v>611.6</v>
+        <f t="shared" si="7"/>
+        <v>596.80000000000007</v>
       </c>
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.25">
@@ -7851,10 +8362,12 @@
         <v>211</v>
       </c>
       <c r="C212">
-        <v>706.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>688.40000000000123</v>
       </c>
       <c r="D212">
-        <v>614.4</v>
+        <f t="shared" si="7"/>
+        <v>599.6</v>
       </c>
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.25">
@@ -7862,10 +8375,12 @@
         <v>212</v>
       </c>
       <c r="C213">
-        <v>710.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>691.60000000000127</v>
       </c>
       <c r="D213">
-        <v>617.20000000000005</v>
+        <f t="shared" si="7"/>
+        <v>602.4</v>
       </c>
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.25">
@@ -7873,10 +8388,12 @@
         <v>213</v>
       </c>
       <c r="C214">
-        <v>713.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>694.80000000000132</v>
       </c>
       <c r="D214">
-        <v>620</v>
+        <f t="shared" si="7"/>
+        <v>605.19999999999993</v>
       </c>
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.25">
@@ -7884,10 +8401,12 @@
         <v>214</v>
       </c>
       <c r="C215">
-        <v>716.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>698.00000000000136</v>
       </c>
       <c r="D215">
-        <v>622.79999999999995</v>
+        <f t="shared" si="7"/>
+        <v>607.99999999999989</v>
       </c>
     </row>
     <row r="216" spans="2:4" x14ac:dyDescent="0.25">
@@ -7895,10 +8414,12 @@
         <v>215</v>
       </c>
       <c r="C216">
-        <v>719.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>701.20000000000141</v>
       </c>
       <c r="D216">
-        <v>625.6</v>
+        <f t="shared" si="7"/>
+        <v>610.79999999999984</v>
       </c>
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.25">
@@ -7906,10 +8427,12 @@
         <v>216</v>
       </c>
       <c r="C217">
-        <v>722.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>704.40000000000146</v>
       </c>
       <c r="D217">
-        <v>628.4</v>
+        <f t="shared" si="7"/>
+        <v>613.5999999999998</v>
       </c>
     </row>
     <row r="218" spans="2:4" x14ac:dyDescent="0.25">
@@ -7917,10 +8440,12 @@
         <v>217</v>
       </c>
       <c r="C218">
-        <v>726.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>707.6000000000015</v>
       </c>
       <c r="D218">
-        <v>631.20000000000005</v>
+        <f t="shared" si="7"/>
+        <v>616.39999999999975</v>
       </c>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.25">
@@ -7928,10 +8453,12 @@
         <v>218</v>
       </c>
       <c r="C219">
-        <v>729.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>710.80000000000155</v>
       </c>
       <c r="D219">
-        <v>634</v>
+        <f t="shared" si="7"/>
+        <v>619.1999999999997</v>
       </c>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.25">
@@ -7939,10 +8466,12 @@
         <v>219</v>
       </c>
       <c r="C220">
-        <v>732.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>714.00000000000159</v>
       </c>
       <c r="D220">
-        <v>636.79999999999995</v>
+        <f t="shared" si="7"/>
+        <v>621.99999999999966</v>
       </c>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
@@ -7950,10 +8479,12 @@
         <v>220</v>
       </c>
       <c r="C221">
-        <v>735.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>717.20000000000164</v>
       </c>
       <c r="D221">
-        <v>639.6</v>
+        <f t="shared" si="7"/>
+        <v>624.79999999999961</v>
       </c>
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.25">
@@ -7961,10 +8492,12 @@
         <v>221</v>
       </c>
       <c r="C222">
-        <v>738.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>720.40000000000168</v>
       </c>
       <c r="D222">
-        <v>642.4</v>
+        <f t="shared" si="7"/>
+        <v>627.59999999999957</v>
       </c>
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.25">
@@ -7972,10 +8505,12 @@
         <v>222</v>
       </c>
       <c r="C223">
-        <v>742.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>723.60000000000173</v>
       </c>
       <c r="D223">
-        <v>645.20000000000005</v>
+        <f t="shared" si="7"/>
+        <v>630.39999999999952</v>
       </c>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.25">
@@ -7983,10 +8518,12 @@
         <v>223</v>
       </c>
       <c r="C224">
-        <v>745.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>726.80000000000177</v>
       </c>
       <c r="D224">
-        <v>648</v>
+        <f t="shared" si="7"/>
+        <v>633.19999999999948</v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
@@ -7994,10 +8531,12 @@
         <v>224</v>
       </c>
       <c r="C225">
-        <v>748.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>730.00000000000182</v>
       </c>
       <c r="D225">
-        <v>650.79999999999995</v>
+        <f t="shared" si="7"/>
+        <v>635.99999999999943</v>
       </c>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
@@ -8005,10 +8544,12 @@
         <v>225</v>
       </c>
       <c r="C226">
-        <v>751.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>733.20000000000186</v>
       </c>
       <c r="D226">
-        <v>653.6</v>
+        <f t="shared" si="7"/>
+        <v>638.79999999999939</v>
       </c>
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.25">
@@ -8016,10 +8557,12 @@
         <v>226</v>
       </c>
       <c r="C227">
-        <v>754.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>736.40000000000191</v>
       </c>
       <c r="D227">
-        <v>656.4</v>
+        <f t="shared" si="7"/>
+        <v>641.59999999999934</v>
       </c>
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.25">
@@ -8027,10 +8570,12 @@
         <v>227</v>
       </c>
       <c r="C228">
-        <v>758.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>739.60000000000196</v>
       </c>
       <c r="D228">
-        <v>659.2</v>
+        <f t="shared" si="7"/>
+        <v>644.3999999999993</v>
       </c>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.25">
@@ -8038,10 +8583,12 @@
         <v>228</v>
       </c>
       <c r="C229">
-        <v>761.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>742.800000000002</v>
       </c>
       <c r="D229">
-        <v>662</v>
+        <f t="shared" si="7"/>
+        <v>647.19999999999925</v>
       </c>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.25">
@@ -8049,10 +8596,12 @@
         <v>229</v>
       </c>
       <c r="C230">
-        <v>764.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>746.00000000000205</v>
       </c>
       <c r="D230">
-        <v>664.8</v>
+        <f t="shared" si="7"/>
+        <v>649.9999999999992</v>
       </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
@@ -8060,10 +8609,12 @@
         <v>230</v>
       </c>
       <c r="C231">
-        <v>767.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>749.20000000000209</v>
       </c>
       <c r="D231">
-        <v>667.6</v>
+        <f t="shared" si="7"/>
+        <v>652.79999999999916</v>
       </c>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.25">
@@ -8071,10 +8622,12 @@
         <v>231</v>
       </c>
       <c r="C232">
-        <v>770.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>752.40000000000214</v>
       </c>
       <c r="D232">
-        <v>670.4</v>
+        <f t="shared" si="7"/>
+        <v>655.59999999999911</v>
       </c>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.25">
@@ -8082,10 +8635,12 @@
         <v>232</v>
       </c>
       <c r="C233">
-        <v>774.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>755.60000000000218</v>
       </c>
       <c r="D233">
-        <v>673.2</v>
+        <f t="shared" si="7"/>
+        <v>658.39999999999907</v>
       </c>
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.25">
@@ -8093,10 +8648,12 @@
         <v>233</v>
       </c>
       <c r="C234">
-        <v>777.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>758.80000000000223</v>
       </c>
       <c r="D234">
-        <v>676</v>
+        <f t="shared" si="7"/>
+        <v>661.19999999999902</v>
       </c>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.25">
@@ -8104,10 +8661,12 @@
         <v>234</v>
       </c>
       <c r="C235">
-        <v>780.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>762.00000000000227</v>
       </c>
       <c r="D235">
-        <v>678.8</v>
+        <f t="shared" si="7"/>
+        <v>663.99999999999898</v>
       </c>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.25">
@@ -8115,10 +8674,12 @@
         <v>235</v>
       </c>
       <c r="C236">
-        <v>783.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>765.20000000000232</v>
       </c>
       <c r="D236">
-        <v>681.6</v>
+        <f t="shared" si="7"/>
+        <v>666.79999999999893</v>
       </c>
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.25">
@@ -8126,10 +8687,12 @@
         <v>236</v>
       </c>
       <c r="C237">
-        <v>786.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>768.40000000000236</v>
       </c>
       <c r="D237">
-        <v>684.4</v>
+        <f t="shared" si="7"/>
+        <v>669.59999999999889</v>
       </c>
     </row>
     <row r="238" spans="2:4" x14ac:dyDescent="0.25">
@@ -8137,10 +8700,12 @@
         <v>237</v>
       </c>
       <c r="C238">
-        <v>790.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>771.60000000000241</v>
       </c>
       <c r="D238">
-        <v>687.2</v>
+        <f t="shared" si="7"/>
+        <v>672.39999999999884</v>
       </c>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.25">
@@ -8148,10 +8713,12 @@
         <v>238</v>
       </c>
       <c r="C239">
-        <v>793.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>774.80000000000246</v>
       </c>
       <c r="D239">
-        <v>690</v>
+        <f t="shared" si="7"/>
+        <v>675.19999999999879</v>
       </c>
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.25">
@@ -8159,10 +8726,12 @@
         <v>239</v>
       </c>
       <c r="C240">
-        <v>796.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>778.0000000000025</v>
       </c>
       <c r="D240">
-        <v>692.8</v>
+        <f t="shared" si="7"/>
+        <v>677.99999999999875</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
@@ -8170,10 +8739,12 @@
         <v>240</v>
       </c>
       <c r="C241">
-        <v>799.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>781.20000000000255</v>
       </c>
       <c r="D241">
-        <v>695.6</v>
+        <f t="shared" si="7"/>
+        <v>680.7999999999987</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
@@ -8181,10 +8752,12 @@
         <v>241</v>
       </c>
       <c r="C242">
-        <v>802.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>784.40000000000259</v>
       </c>
       <c r="D242">
-        <v>698.4</v>
+        <f t="shared" si="7"/>
+        <v>683.59999999999866</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
@@ -8192,10 +8765,12 @@
         <v>242</v>
       </c>
       <c r="C243">
-        <v>806.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>787.60000000000264</v>
       </c>
       <c r="D243">
-        <v>701.2</v>
+        <f t="shared" si="7"/>
+        <v>686.39999999999861</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
@@ -8203,10 +8778,12 @@
         <v>243</v>
       </c>
       <c r="C244">
-        <v>809.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>790.80000000000268</v>
       </c>
       <c r="D244">
-        <v>704</v>
+        <f t="shared" si="7"/>
+        <v>689.19999999999857</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
@@ -8214,10 +8791,12 @@
         <v>244</v>
       </c>
       <c r="C245">
-        <v>812.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>794.00000000000273</v>
       </c>
       <c r="D245">
-        <v>706.8</v>
+        <f t="shared" si="7"/>
+        <v>691.99999999999852</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
@@ -8225,10 +8804,12 @@
         <v>245</v>
       </c>
       <c r="C246">
-        <v>815.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>797.20000000000277</v>
       </c>
       <c r="D246">
-        <v>709.6</v>
+        <f t="shared" si="7"/>
+        <v>694.79999999999848</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
@@ -8236,10 +8817,12 @@
         <v>246</v>
       </c>
       <c r="C247">
-        <v>818.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>800.40000000000282</v>
       </c>
       <c r="D247">
-        <v>712.4</v>
+        <f t="shared" si="7"/>
+        <v>697.59999999999843</v>
       </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
@@ -8247,10 +8830,12 @@
         <v>247</v>
       </c>
       <c r="C248">
-        <v>822.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>803.60000000000286</v>
       </c>
       <c r="D248">
-        <v>715.2</v>
+        <f t="shared" si="7"/>
+        <v>700.39999999999839</v>
       </c>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.25">
@@ -8258,10 +8843,12 @@
         <v>248</v>
       </c>
       <c r="C249">
-        <v>825.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>806.80000000000291</v>
       </c>
       <c r="D249">
-        <v>718</v>
+        <f t="shared" si="7"/>
+        <v>703.19999999999834</v>
       </c>
     </row>
     <row r="250" spans="2:4" x14ac:dyDescent="0.25">
@@ -8269,10 +8856,12 @@
         <v>249</v>
       </c>
       <c r="C250">
-        <v>828.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>810.00000000000296</v>
       </c>
       <c r="D250">
-        <v>720.8</v>
+        <f t="shared" si="7"/>
+        <v>705.99999999999829</v>
       </c>
     </row>
     <row r="251" spans="2:4" x14ac:dyDescent="0.25">
@@ -8280,10 +8869,12 @@
         <v>250</v>
       </c>
       <c r="C251">
-        <v>831.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>813.200000000003</v>
       </c>
       <c r="D251">
-        <v>723.6</v>
+        <f t="shared" si="7"/>
+        <v>708.79999999999825</v>
       </c>
     </row>
     <row r="252" spans="2:4" x14ac:dyDescent="0.25">
@@ -8291,10 +8882,12 @@
         <v>251</v>
       </c>
       <c r="C252">
-        <v>834.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>816.40000000000305</v>
       </c>
       <c r="D252">
-        <v>726.4</v>
+        <f t="shared" si="7"/>
+        <v>711.5999999999982</v>
       </c>
     </row>
     <row r="253" spans="2:4" x14ac:dyDescent="0.25">
@@ -8302,10 +8895,12 @@
         <v>252</v>
       </c>
       <c r="C253">
-        <v>838.00000000000102</v>
+        <f t="shared" si="6"/>
+        <v>819.60000000000309</v>
       </c>
       <c r="D253">
-        <v>729.2</v>
+        <f t="shared" si="7"/>
+        <v>714.39999999999816</v>
       </c>
     </row>
     <row r="254" spans="2:4" x14ac:dyDescent="0.25">
@@ -8313,10 +8908,12 @@
         <v>253</v>
       </c>
       <c r="C254">
-        <v>841.20000000000095</v>
+        <f t="shared" si="6"/>
+        <v>822.80000000000314</v>
       </c>
       <c r="D254">
-        <v>732</v>
+        <f t="shared" si="7"/>
+        <v>717.19999999999811</v>
       </c>
     </row>
     <row r="255" spans="2:4" x14ac:dyDescent="0.25">
@@ -8324,10 +8921,12 @@
         <v>254</v>
       </c>
       <c r="C255">
-        <v>844.400000000001</v>
+        <f t="shared" si="6"/>
+        <v>826.00000000000318</v>
       </c>
       <c r="D255">
-        <v>734.8</v>
+        <f t="shared" si="7"/>
+        <v>719.99999999999807</v>
       </c>
     </row>
     <row r="256" spans="2:4" x14ac:dyDescent="0.25">
@@ -8335,10 +8934,12 @@
         <v>255</v>
       </c>
       <c r="C256">
-        <v>847.60000000000105</v>
+        <f t="shared" si="6"/>
+        <v>829.20000000000323</v>
       </c>
       <c r="D256">
-        <v>737.6</v>
+        <f t="shared" si="7"/>
+        <v>722.79999999999802</v>
       </c>
     </row>
     <row r="257" spans="2:4" x14ac:dyDescent="0.25">
@@ -8346,10 +8947,12 @@
         <v>256</v>
       </c>
       <c r="C257">
-        <v>850.80000000000098</v>
+        <f t="shared" si="6"/>
+        <v>832.40000000000327</v>
       </c>
       <c r="D257">
-        <v>740.4</v>
+        <f t="shared" si="7"/>
+        <v>725.59999999999798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>